<commit_message>
Selected two use cases and estimated LOC and Minutes
</commit_message>
<xml_diff>
--- a/TeamEstherKarelKeithTroyReport.xlsx
+++ b/TeamEstherKarelKeithTroyReport.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18827"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klros\Google Drive\Keith\Stevens Institute of Technology\SSW-555-WS\Projects\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="38400" windowHeight="20020" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -20,20 +25,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backlog!$A$1:$H$1</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="194">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -644,7 +649,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -882,7 +887,7 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="68"/>
+    <cellStyle name="Normal 2" xfId="68" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -898,7 +903,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -924,22 +929,22 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41065.0</c:v>
+                  <c:v>41065</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41078.0</c:v>
+                  <c:v>41078</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41092.0</c:v>
+                  <c:v>41092</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41106.0</c:v>
+                  <c:v>41106</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41120.0</c:v>
+                  <c:v>41120</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -951,25 +956,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8005-41C3-A2A6-994BE20B6C54}"/>
             </c:ext>
@@ -995,7 +1000,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1028,14 +1033,14 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1064,10 +1069,10 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>40442.0</c:v>
+                  <c:v>40442</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40455.0</c:v>
+                  <c:v>40455</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1079,16 +1084,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>36.0</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5A9F-42BD-9352-89747C7C9AC0}"/>
             </c:ext>
@@ -1147,7 +1152,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1173,7 +1178,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1211,7 +1216,7 @@
         <xdr:cNvPr id="3" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1286,7 +1291,7 @@
         <xdr:cNvPr id="4" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1351,7 +1356,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1420,7 +1425,7 @@
         <xdr:cNvPr id="6" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1490,7 +1495,7 @@
         <xdr:cNvPr id="7" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1559,7 +1564,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1629,7 +1634,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1969,22 +1974,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="7.87890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.41015625" customWidth="1"/>
+    <col min="3" max="3" width="10.87890625" customWidth="1"/>
+    <col min="4" max="4" width="20.41015625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -1998,7 +2003,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>172</v>
       </c>
@@ -2012,7 +2017,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>179</v>
       </c>
@@ -2026,7 +2031,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>184</v>
       </c>
@@ -2040,7 +2045,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>191</v>
       </c>
@@ -2054,7 +2059,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>192</v>
       </c>
@@ -2068,7 +2073,7 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1"/>
+    <hyperlink ref="D9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2081,19 +2086,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="150" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.703125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="29.42578125" customWidth="1"/>
+    <col min="5" max="5" width="29.41015625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>177</v>
       </c>
@@ -2122,7 +2127,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30">
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.3">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -2143,7 +2148,7 @@
       <c r="H2" s="19"/>
       <c r="I2" s="18"/>
     </row>
-    <row r="3" spans="1:9" ht="45">
+    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.3">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -2164,7 +2169,7 @@
       <c r="H3" s="19"/>
       <c r="I3" s="18"/>
     </row>
-    <row r="4" spans="1:9" ht="30">
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.3">
       <c r="A4" s="18">
         <v>3</v>
       </c>
@@ -2185,7 +2190,7 @@
       <c r="H4" s="19"/>
       <c r="I4" s="18"/>
     </row>
-    <row r="5" spans="1:9" ht="45">
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.3">
       <c r="A5" s="18">
         <v>4</v>
       </c>
@@ -2206,7 +2211,7 @@
       <c r="H5" s="19"/>
       <c r="I5" s="18"/>
     </row>
-    <row r="6" spans="1:9" ht="30">
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.3">
       <c r="A6" s="18">
         <v>5</v>
       </c>
@@ -2227,7 +2232,7 @@
       <c r="H6" s="19"/>
       <c r="I6" s="18"/>
     </row>
-    <row r="7" spans="1:9" ht="30">
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.3">
       <c r="A7" s="18">
         <v>6</v>
       </c>
@@ -2248,7 +2253,7 @@
       <c r="H7" s="19"/>
       <c r="I7" s="18"/>
     </row>
-    <row r="8" spans="1:9" ht="60">
+    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.3">
       <c r="A8" s="18">
         <v>7</v>
       </c>
@@ -2269,7 +2274,7 @@
       <c r="H8" s="19"/>
       <c r="I8" s="18"/>
     </row>
-    <row r="9" spans="1:9" ht="30">
+    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.3">
       <c r="A9" s="18">
         <v>8</v>
       </c>
@@ -2290,7 +2295,7 @@
       <c r="H9" s="19"/>
       <c r="I9" s="18"/>
     </row>
-    <row r="10" spans="1:9" ht="45">
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="18"/>
       <c r="C10" s="18" t="s">
@@ -2307,7 +2312,7 @@
       <c r="H10" s="19"/>
       <c r="I10" s="18"/>
     </row>
-    <row r="11" spans="1:9" ht="30">
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
       <c r="C11" s="18" t="s">
@@ -2324,7 +2329,7 @@
       <c r="H11" s="19"/>
       <c r="I11" s="18"/>
     </row>
-    <row r="12" spans="1:9" ht="30">
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="18"/>
       <c r="C12" s="18" t="s">
@@ -2341,7 +2346,7 @@
       <c r="H12" s="19"/>
       <c r="I12" s="18"/>
     </row>
-    <row r="13" spans="1:9" ht="45">
+    <row r="13" spans="1:9" ht="60" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
       <c r="C13" s="18" t="s">
@@ -2358,7 +2363,7 @@
       <c r="H13" s="19"/>
       <c r="I13" s="18"/>
     </row>
-    <row r="14" spans="1:9" ht="45">
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.3">
       <c r="A14" s="18"/>
       <c r="B14" s="18"/>
       <c r="C14" s="18" t="s">
@@ -2375,7 +2380,7 @@
       <c r="H14" s="19"/>
       <c r="I14" s="18"/>
     </row>
-    <row r="15" spans="1:9" ht="45">
+    <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.3">
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
       <c r="C15" s="18" t="s">
@@ -2392,7 +2397,7 @@
       <c r="H15" s="19"/>
       <c r="I15" s="18"/>
     </row>
-    <row r="16" spans="1:9" ht="30">
+    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
       <c r="B16" s="18"/>
       <c r="C16" s="18" t="s">
@@ -2409,7 +2414,7 @@
       <c r="H16" s="19"/>
       <c r="I16" s="18"/>
     </row>
-    <row r="17" spans="3:8" ht="60">
+    <row r="17" spans="3:8" ht="60" x14ac:dyDescent="0.3">
       <c r="C17" s="18" t="s">
         <v>118</v>
       </c>
@@ -2423,7 +2428,7 @@
       <c r="G17" s="19"/>
       <c r="H17" s="19"/>
     </row>
-    <row r="18" spans="3:8" ht="90">
+    <row r="18" spans="3:8" ht="90" x14ac:dyDescent="0.3">
       <c r="C18" s="18" t="s">
         <v>119</v>
       </c>
@@ -2437,7 +2442,7 @@
       <c r="G18" s="19"/>
       <c r="H18" s="19"/>
     </row>
-    <row r="19" spans="3:8" ht="30">
+    <row r="19" spans="3:8" ht="30" x14ac:dyDescent="0.3">
       <c r="C19" s="18" t="s">
         <v>120</v>
       </c>
@@ -2451,7 +2456,7 @@
       <c r="G19" s="19"/>
       <c r="H19" s="19"/>
     </row>
-    <row r="20" spans="3:8" ht="30">
+    <row r="20" spans="3:8" ht="30" x14ac:dyDescent="0.3">
       <c r="C20" s="18" t="s">
         <v>121</v>
       </c>
@@ -2465,7 +2470,7 @@
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
     </row>
-    <row r="21" spans="3:8" ht="30">
+    <row r="21" spans="3:8" ht="30" x14ac:dyDescent="0.3">
       <c r="C21" s="18" t="s">
         <v>123</v>
       </c>
@@ -2479,7 +2484,7 @@
       <c r="G21" s="19"/>
       <c r="H21" s="19"/>
     </row>
-    <row r="22" spans="3:8" ht="30">
+    <row r="22" spans="3:8" ht="30" x14ac:dyDescent="0.3">
       <c r="C22" s="18" t="s">
         <v>124</v>
       </c>
@@ -2493,7 +2498,7 @@
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
     </row>
-    <row r="23" spans="3:8" ht="30">
+    <row r="23" spans="3:8" ht="30" x14ac:dyDescent="0.3">
       <c r="C23" s="18" t="s">
         <v>125</v>
       </c>
@@ -2507,7 +2512,7 @@
       <c r="G23" s="19"/>
       <c r="H23" s="19"/>
     </row>
-    <row r="24" spans="3:8" ht="30">
+    <row r="24" spans="3:8" ht="30" x14ac:dyDescent="0.3">
       <c r="C24" s="18" t="s">
         <v>126</v>
       </c>
@@ -2521,7 +2526,7 @@
       <c r="G24" s="19"/>
       <c r="H24" s="19"/>
     </row>
-    <row r="25" spans="3:8" ht="60">
+    <row r="25" spans="3:8" ht="60" x14ac:dyDescent="0.3">
       <c r="C25" s="18" t="s">
         <v>130</v>
       </c>
@@ -2535,7 +2540,7 @@
       <c r="G25" s="19"/>
       <c r="H25" s="19"/>
     </row>
-    <row r="26" spans="3:8" ht="45">
+    <row r="26" spans="3:8" ht="45" x14ac:dyDescent="0.3">
       <c r="C26" s="18" t="s">
         <v>131</v>
       </c>
@@ -2549,7 +2554,7 @@
       <c r="G26" s="19"/>
       <c r="H26" s="19"/>
     </row>
-    <row r="27" spans="3:8" ht="165">
+    <row r="27" spans="3:8" ht="195" x14ac:dyDescent="0.3">
       <c r="C27" s="18" t="s">
         <v>132</v>
       </c>
@@ -2563,7 +2568,7 @@
       <c r="G27" s="19"/>
       <c r="H27" s="19"/>
     </row>
-    <row r="28" spans="3:8" ht="30">
+    <row r="28" spans="3:8" ht="30" x14ac:dyDescent="0.3">
       <c r="C28" s="18" t="s">
         <v>133</v>
       </c>
@@ -2577,7 +2582,7 @@
       <c r="G28" s="19"/>
       <c r="H28" s="19"/>
     </row>
-    <row r="29" spans="3:8" ht="45">
+    <row r="29" spans="3:8" ht="45" x14ac:dyDescent="0.3">
       <c r="C29" s="18" t="s">
         <v>134</v>
       </c>
@@ -2591,7 +2596,7 @@
       <c r="G29" s="19"/>
       <c r="H29" s="19"/>
     </row>
-    <row r="30" spans="3:8" ht="30">
+    <row r="30" spans="3:8" ht="30" x14ac:dyDescent="0.3">
       <c r="C30" s="18" t="s">
         <v>135</v>
       </c>
@@ -2605,7 +2610,7 @@
       <c r="G30" s="19"/>
       <c r="H30" s="19"/>
     </row>
-    <row r="31" spans="3:8" ht="30">
+    <row r="31" spans="3:8" ht="30" x14ac:dyDescent="0.3">
       <c r="C31" s="18" t="s">
         <v>136</v>
       </c>
@@ -2619,7 +2624,7 @@
       <c r="G31" s="19"/>
       <c r="H31" s="19"/>
     </row>
-    <row r="32" spans="3:8" ht="45">
+    <row r="32" spans="3:8" ht="45" x14ac:dyDescent="0.3">
       <c r="C32" s="18" t="s">
         <v>137</v>
       </c>
@@ -2633,7 +2638,7 @@
       <c r="G32" s="19"/>
       <c r="H32" s="19"/>
     </row>
-    <row r="33" spans="3:8" ht="30">
+    <row r="33" spans="3:8" ht="30" x14ac:dyDescent="0.3">
       <c r="C33" s="18" t="s">
         <v>138</v>
       </c>
@@ -2648,7 +2653,7 @@
       <c r="H33" s="19"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1"/>
+  <autoFilter ref="A1:H1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2661,54 +2666,54 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="7"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="9.41015625" customWidth="1"/>
+    <col min="3" max="3" width="15.87890625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.29296875" customWidth="1"/>
+    <col min="5" max="5" width="6.87890625" customWidth="1"/>
+    <col min="6" max="6" width="12.41015625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>154</v>
       </c>
@@ -2731,7 +2736,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>155</v>
       </c>
@@ -2747,7 +2752,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>156</v>
       </c>
@@ -2772,7 +2777,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>157</v>
       </c>
@@ -2797,7 +2802,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>158</v>
       </c>
@@ -2822,7 +2827,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>159</v>
       </c>
@@ -2860,24 +2865,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="2"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="16.703125" customWidth="1"/>
+    <col min="3" max="3" width="12.41015625" customWidth="1"/>
+    <col min="4" max="4" width="7.1171875" customWidth="1"/>
+    <col min="5" max="5" width="6.87890625" customWidth="1"/>
+    <col min="6" max="6" width="12.41015625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2897,7 +2902,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>40442</v>
       </c>
@@ -2908,7 +2913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>40455</v>
       </c>
@@ -2944,26 +2949,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="7.703125" customWidth="1"/>
+    <col min="2" max="2" width="24.41015625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.703125" customWidth="1"/>
+    <col min="5" max="5" width="9.29296875" customWidth="1"/>
+    <col min="6" max="6" width="10.41015625" customWidth="1"/>
+    <col min="7" max="7" width="9.1171875" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="11.29296875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2992,7 +2995,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>128</v>
       </c>
@@ -3003,15 +3006,24 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>129</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="C3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E3">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>122</v>
       </c>
@@ -3022,7 +3034,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>107</v>
       </c>
@@ -3030,7 +3042,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>108</v>
       </c>
@@ -3038,7 +3050,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>109</v>
       </c>
@@ -3049,7 +3061,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>113</v>
       </c>
@@ -3060,29 +3072,38 @@
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>127</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="C9" t="s">
+        <v>184</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" s="5"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="2:2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>26</v>
       </c>
@@ -3100,16 +3121,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3151,16 +3172,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3201,16 +3222,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3251,20 +3272,20 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C33" sqref="A2:C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1171875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.41015625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>106</v>
       </c>
@@ -3275,7 +3296,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -3286,7 +3307,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -3297,7 +3318,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -3308,7 +3329,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -3319,7 +3340,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>111</v>
       </c>
@@ -3330,7 +3351,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -3341,7 +3362,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>113</v>
       </c>
@@ -3352,7 +3373,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -3363,7 +3384,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>115</v>
       </c>
@@ -3374,7 +3395,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>116</v>
       </c>
@@ -3385,7 +3406,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>117</v>
       </c>
@@ -3396,7 +3417,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>118</v>
       </c>
@@ -3407,7 +3428,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="45">
+    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>119</v>
       </c>
@@ -3418,7 +3439,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15">
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>120</v>
       </c>
@@ -3429,7 +3450,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>121</v>
       </c>
@@ -3440,7 +3461,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>122</v>
       </c>
@@ -3451,7 +3472,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>123</v>
       </c>
@@ -3462,7 +3483,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>124</v>
       </c>
@@ -3473,7 +3494,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>125</v>
       </c>
@@ -3484,7 +3505,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>126</v>
       </c>
@@ -3495,7 +3516,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>127</v>
       </c>
@@ -3506,7 +3527,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>128</v>
       </c>
@@ -3517,7 +3538,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>129</v>
       </c>
@@ -3528,7 +3549,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>130</v>
       </c>
@@ -3539,7 +3560,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>131</v>
       </c>
@@ -3550,7 +3571,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="90">
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>132</v>
       </c>
@@ -3561,7 +3582,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>133</v>
       </c>
@@ -3572,7 +3593,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>134</v>
       </c>
@@ -3583,7 +3604,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>135</v>
       </c>
@@ -3594,7 +3615,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>136</v>
       </c>
@@ -3605,7 +3626,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>137</v>
       </c>
@@ -3616,7 +3637,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>138</v>
       </c>
@@ -3627,7 +3648,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>139</v>
       </c>
@@ -3638,7 +3659,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>140</v>
       </c>
@@ -3649,7 +3670,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>141</v>
       </c>
@@ -3660,7 +3681,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15">
+    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>142</v>
       </c>
@@ -3671,7 +3692,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>143</v>
       </c>
@@ -3682,7 +3703,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>144</v>
       </c>
@@ -3693,7 +3714,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>145</v>
       </c>
@@ -3704,7 +3725,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>146</v>
       </c>
@@ -3715,7 +3736,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>147</v>
       </c>
@@ -3726,7 +3747,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>148</v>
       </c>

</xml_diff>

<commit_message>
updated sprint 1 estimates
updated sprint 1 estimates for ej stories
</commit_message>
<xml_diff>
--- a/TeamEstherKarelKeithTroyReport.xlsx
+++ b/TeamEstherKarelKeithTroyReport.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18827"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klros\Google Drive\Keith\Stevens Institute of Technology\SSW-555-WS\Projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esthe\OneDrive\Documents\GitHub\stevens_cs555\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backlog!$A$1:$H$1</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -649,7 +649,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -887,7 +887,7 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="68" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
+    <cellStyle name="Normal 2" xfId="68"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1974,22 +1974,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.87890625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.41015625" customWidth="1"/>
-    <col min="3" max="3" width="10.87890625" customWidth="1"/>
-    <col min="4" max="4" width="20.41015625" customWidth="1"/>
+    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.375" customWidth="1"/>
+    <col min="3" max="3" width="10.875" customWidth="1"/>
+    <col min="4" max="4" width="20.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>172</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>179</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>184</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>191</v>
       </c>
@@ -2059,7 +2059,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>192</v>
       </c>
@@ -2073,7 +2073,7 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D9" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2086,19 +2086,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="150" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.703125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="29.41015625" customWidth="1"/>
+    <col min="5" max="5" width="29.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>177</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -2148,7 +2148,7 @@
       <c r="H2" s="19"/>
       <c r="I2" s="18"/>
     </row>
-    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="63" x14ac:dyDescent="0.2">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -2169,7 +2169,7 @@
       <c r="H3" s="19"/>
       <c r="I3" s="18"/>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A4" s="18">
         <v>3</v>
       </c>
@@ -2190,7 +2190,7 @@
       <c r="H4" s="19"/>
       <c r="I4" s="18"/>
     </row>
-    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A5" s="18">
         <v>4</v>
       </c>
@@ -2211,7 +2211,7 @@
       <c r="H5" s="19"/>
       <c r="I5" s="18"/>
     </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A6" s="18">
         <v>5</v>
       </c>
@@ -2232,7 +2232,7 @@
       <c r="H6" s="19"/>
       <c r="I6" s="18"/>
     </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A7" s="18">
         <v>6</v>
       </c>
@@ -2253,7 +2253,7 @@
       <c r="H7" s="19"/>
       <c r="I7" s="18"/>
     </row>
-    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="78.75" x14ac:dyDescent="0.2">
       <c r="A8" s="18">
         <v>7</v>
       </c>
@@ -2274,7 +2274,7 @@
       <c r="H8" s="19"/>
       <c r="I8" s="18"/>
     </row>
-    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A9" s="18">
         <v>8</v>
       </c>
@@ -2295,7 +2295,7 @@
       <c r="H9" s="19"/>
       <c r="I9" s="18"/>
     </row>
-    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="63" x14ac:dyDescent="0.2">
       <c r="A10" s="18"/>
       <c r="B10" s="18"/>
       <c r="C10" s="18" t="s">
@@ -2312,7 +2312,7 @@
       <c r="H10" s="19"/>
       <c r="I10" s="18"/>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
       <c r="C11" s="18" t="s">
@@ -2329,7 +2329,7 @@
       <c r="H11" s="19"/>
       <c r="I11" s="18"/>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A12" s="18"/>
       <c r="B12" s="18"/>
       <c r="C12" s="18" t="s">
@@ -2346,7 +2346,7 @@
       <c r="H12" s="19"/>
       <c r="I12" s="18"/>
     </row>
-    <row r="13" spans="1:9" ht="60" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="63" x14ac:dyDescent="0.2">
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
       <c r="C13" s="18" t="s">
@@ -2363,7 +2363,7 @@
       <c r="H13" s="19"/>
       <c r="I13" s="18"/>
     </row>
-    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A14" s="18"/>
       <c r="B14" s="18"/>
       <c r="C14" s="18" t="s">
@@ -2380,7 +2380,7 @@
       <c r="H14" s="19"/>
       <c r="I14" s="18"/>
     </row>
-    <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="63" x14ac:dyDescent="0.2">
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
       <c r="C15" s="18" t="s">
@@ -2397,7 +2397,7 @@
       <c r="H15" s="19"/>
       <c r="I15" s="18"/>
     </row>
-    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A16" s="18"/>
       <c r="B16" s="18"/>
       <c r="C16" s="18" t="s">
@@ -2414,7 +2414,7 @@
       <c r="H16" s="19"/>
       <c r="I16" s="18"/>
     </row>
-    <row r="17" spans="3:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:8" ht="78.75" x14ac:dyDescent="0.2">
       <c r="C17" s="18" t="s">
         <v>118</v>
       </c>
@@ -2428,7 +2428,7 @@
       <c r="G17" s="19"/>
       <c r="H17" s="19"/>
     </row>
-    <row r="18" spans="3:8" ht="90" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:8" ht="110.25" x14ac:dyDescent="0.2">
       <c r="C18" s="18" t="s">
         <v>119</v>
       </c>
@@ -2442,7 +2442,7 @@
       <c r="G18" s="19"/>
       <c r="H18" s="19"/>
     </row>
-    <row r="19" spans="3:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:8" ht="47.25" x14ac:dyDescent="0.2">
       <c r="C19" s="18" t="s">
         <v>120</v>
       </c>
@@ -2456,7 +2456,7 @@
       <c r="G19" s="19"/>
       <c r="H19" s="19"/>
     </row>
-    <row r="20" spans="3:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:8" ht="31.5" x14ac:dyDescent="0.2">
       <c r="C20" s="18" t="s">
         <v>121</v>
       </c>
@@ -2470,7 +2470,7 @@
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
     </row>
-    <row r="21" spans="3:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:8" ht="31.5" x14ac:dyDescent="0.2">
       <c r="C21" s="18" t="s">
         <v>123</v>
       </c>
@@ -2484,7 +2484,7 @@
       <c r="G21" s="19"/>
       <c r="H21" s="19"/>
     </row>
-    <row r="22" spans="3:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:8" ht="31.5" x14ac:dyDescent="0.2">
       <c r="C22" s="18" t="s">
         <v>124</v>
       </c>
@@ -2498,7 +2498,7 @@
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
     </row>
-    <row r="23" spans="3:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:8" ht="31.5" x14ac:dyDescent="0.2">
       <c r="C23" s="18" t="s">
         <v>125</v>
       </c>
@@ -2512,7 +2512,7 @@
       <c r="G23" s="19"/>
       <c r="H23" s="19"/>
     </row>
-    <row r="24" spans="3:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:8" ht="47.25" x14ac:dyDescent="0.2">
       <c r="C24" s="18" t="s">
         <v>126</v>
       </c>
@@ -2526,7 +2526,7 @@
       <c r="G24" s="19"/>
       <c r="H24" s="19"/>
     </row>
-    <row r="25" spans="3:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:8" ht="78.75" x14ac:dyDescent="0.2">
       <c r="C25" s="18" t="s">
         <v>130</v>
       </c>
@@ -2540,7 +2540,7 @@
       <c r="G25" s="19"/>
       <c r="H25" s="19"/>
     </row>
-    <row r="26" spans="3:8" ht="45" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:8" ht="47.25" x14ac:dyDescent="0.2">
       <c r="C26" s="18" t="s">
         <v>131</v>
       </c>
@@ -2554,7 +2554,7 @@
       <c r="G26" s="19"/>
       <c r="H26" s="19"/>
     </row>
-    <row r="27" spans="3:8" ht="195" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:8" ht="204.75" x14ac:dyDescent="0.2">
       <c r="C27" s="18" t="s">
         <v>132</v>
       </c>
@@ -2568,7 +2568,7 @@
       <c r="G27" s="19"/>
       <c r="H27" s="19"/>
     </row>
-    <row r="28" spans="3:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:8" ht="31.5" x14ac:dyDescent="0.2">
       <c r="C28" s="18" t="s">
         <v>133</v>
       </c>
@@ -2582,7 +2582,7 @@
       <c r="G28" s="19"/>
       <c r="H28" s="19"/>
     </row>
-    <row r="29" spans="3:8" ht="45" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:8" ht="47.25" x14ac:dyDescent="0.2">
       <c r="C29" s="18" t="s">
         <v>134</v>
       </c>
@@ -2596,7 +2596,7 @@
       <c r="G29" s="19"/>
       <c r="H29" s="19"/>
     </row>
-    <row r="30" spans="3:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:8" ht="31.5" x14ac:dyDescent="0.2">
       <c r="C30" s="18" t="s">
         <v>135</v>
       </c>
@@ -2610,7 +2610,7 @@
       <c r="G30" s="19"/>
       <c r="H30" s="19"/>
     </row>
-    <row r="31" spans="3:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:8" ht="31.5" x14ac:dyDescent="0.2">
       <c r="C31" s="18" t="s">
         <v>136</v>
       </c>
@@ -2624,7 +2624,7 @@
       <c r="G31" s="19"/>
       <c r="H31" s="19"/>
     </row>
-    <row r="32" spans="3:8" ht="45" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:8" ht="47.25" x14ac:dyDescent="0.2">
       <c r="C32" s="18" t="s">
         <v>137</v>
       </c>
@@ -2638,7 +2638,7 @@
       <c r="G32" s="19"/>
       <c r="H32" s="19"/>
     </row>
-    <row r="33" spans="3:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:8" ht="31.5" x14ac:dyDescent="0.2">
       <c r="C33" s="18" t="s">
         <v>138</v>
       </c>
@@ -2653,7 +2653,7 @@
       <c r="H33" s="19"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:H1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2666,54 +2666,54 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="7"/>
-    <col min="2" max="2" width="9.41015625" customWidth="1"/>
-    <col min="3" max="3" width="15.87890625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.29296875" customWidth="1"/>
-    <col min="5" max="5" width="6.87890625" customWidth="1"/>
-    <col min="6" max="6" width="12.41015625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="9.375" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.25" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="12.375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>154</v>
       </c>
@@ -2736,7 +2736,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>155</v>
       </c>
@@ -2752,7 +2752,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>156</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>157</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>158</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>159</v>
       </c>
@@ -2865,24 +2865,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="2"/>
-    <col min="2" max="2" width="16.703125" customWidth="1"/>
-    <col min="3" max="3" width="12.41015625" customWidth="1"/>
-    <col min="4" max="4" width="7.1171875" customWidth="1"/>
-    <col min="5" max="5" width="6.87890625" customWidth="1"/>
-    <col min="6" max="6" width="12.41015625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="16.75" customWidth="1"/>
+    <col min="3" max="3" width="12.375" customWidth="1"/>
+    <col min="4" max="4" width="7.125" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="12.375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2902,7 +2902,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>40442</v>
       </c>
@@ -2913,7 +2913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>40455</v>
       </c>
@@ -2949,24 +2949,26 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.703125" customWidth="1"/>
-    <col min="2" max="2" width="24.41015625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.703125" customWidth="1"/>
-    <col min="5" max="5" width="9.29296875" customWidth="1"/>
-    <col min="6" max="6" width="10.41015625" customWidth="1"/>
-    <col min="7" max="7" width="9.1171875" customWidth="1"/>
+    <col min="1" max="1" width="7.75" customWidth="1"/>
+    <col min="2" max="2" width="24.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.75" customWidth="1"/>
+    <col min="5" max="5" width="9.25" customWidth="1"/>
+    <col min="6" max="6" width="10.375" customWidth="1"/>
+    <col min="7" max="7" width="9.125" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="11.29296875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="11.25" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2995,7 +2997,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>128</v>
       </c>
@@ -3006,7 +3008,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
         <v>129</v>
       </c>
@@ -3023,7 +3025,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>122</v>
       </c>
@@ -3033,8 +3035,14 @@
       <c r="C4" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
         <v>107</v>
       </c>
@@ -3042,7 +3050,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
         <v>108</v>
       </c>
@@ -3050,7 +3058,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
         <v>109</v>
       </c>
@@ -3061,7 +3069,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
         <v>113</v>
       </c>
@@ -3071,8 +3079,14 @@
       <c r="C8" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
         <v>127</v>
       </c>
@@ -3089,21 +3103,21 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="5"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
         <v>26</v>
       </c>
@@ -3121,16 +3135,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3172,16 +3186,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3222,16 +3236,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3272,20 +3286,20 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C33" sqref="A2:C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.1171875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.41015625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>106</v>
       </c>
@@ -3296,7 +3310,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -3307,7 +3321,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -3318,7 +3332,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -3329,7 +3343,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -3340,7 +3354,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>111</v>
       </c>
@@ -3351,7 +3365,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -3362,7 +3376,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>113</v>
       </c>
@@ -3373,7 +3387,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -3384,7 +3398,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>115</v>
       </c>
@@ -3395,7 +3409,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>116</v>
       </c>
@@ -3406,7 +3420,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>117</v>
       </c>
@@ -3417,7 +3431,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>118</v>
       </c>
@@ -3428,7 +3442,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>119</v>
       </c>
@@ -3439,7 +3453,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>120</v>
       </c>
@@ -3450,7 +3464,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>121</v>
       </c>
@@ -3461,7 +3475,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>122</v>
       </c>
@@ -3472,7 +3486,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>123</v>
       </c>
@@ -3483,7 +3497,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>124</v>
       </c>
@@ -3494,7 +3508,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>125</v>
       </c>
@@ -3505,7 +3519,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>126</v>
       </c>
@@ -3516,7 +3530,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>127</v>
       </c>
@@ -3527,7 +3541,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>128</v>
       </c>
@@ -3538,7 +3552,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>129</v>
       </c>
@@ -3549,7 +3563,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>130</v>
       </c>
@@ -3560,7 +3574,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>131</v>
       </c>
@@ -3571,7 +3585,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="126" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>132</v>
       </c>
@@ -3582,7 +3596,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>133</v>
       </c>
@@ -3593,7 +3607,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>134</v>
       </c>
@@ -3604,7 +3618,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>135</v>
       </c>
@@ -3615,7 +3629,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>136</v>
       </c>
@@ -3626,7 +3640,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>137</v>
       </c>
@@ -3637,7 +3651,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>138</v>
       </c>
@@ -3648,7 +3662,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>139</v>
       </c>
@@ -3659,7 +3673,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>140</v>
       </c>
@@ -3670,7 +3684,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>141</v>
       </c>
@@ -3681,7 +3695,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>142</v>
       </c>
@@ -3692,7 +3706,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>143</v>
       </c>
@@ -3703,7 +3717,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>144</v>
       </c>
@@ -3714,7 +3728,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>145</v>
       </c>
@@ -3725,7 +3739,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>146</v>
       </c>
@@ -3736,7 +3750,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>147</v>
       </c>
@@ -3747,7 +3761,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>148</v>
       </c>

</xml_diff>

<commit_message>
Updated for P03 Assignment
Updated in accordance with the HowToUseTeamXXReport file on Canvas for Sprint 1 and Project 03.
</commit_message>
<xml_diff>
--- a/TeamEstherKarelKeithTroyReport.xlsx
+++ b/TeamEstherKarelKeithTroyReport.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18827"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esthe\OneDrive\Documents\GitHub\stevens_cs555\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klros\Google Drive\Keith\Stevens Institute of Technology\SSW-555-WS\Projects\cs555\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" tabRatio="627" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backlog!$A$1:$H$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="194">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -649,7 +649,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -887,7 +887,7 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="68"/>
+    <cellStyle name="Normal 2" xfId="68" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1069,10 +1069,7 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>40442</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>40455</c:v>
+                  <c:v>41676</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1084,10 +1081,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1974,22 +1968,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.375" customWidth="1"/>
-    <col min="3" max="3" width="10.875" customWidth="1"/>
-    <col min="4" max="4" width="20.375" customWidth="1"/>
+    <col min="1" max="1" width="7.87890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.3515625" customWidth="1"/>
+    <col min="3" max="3" width="10.87890625" customWidth="1"/>
+    <col min="4" max="4" width="20.3515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -2003,7 +1995,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>172</v>
       </c>
@@ -2017,7 +2009,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>179</v>
       </c>
@@ -2031,7 +2023,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>184</v>
       </c>
@@ -2045,7 +2037,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>191</v>
       </c>
@@ -2059,7 +2051,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>192</v>
       </c>
@@ -2073,7 +2065,7 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1"/>
+    <hyperlink ref="D9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2086,19 +2078,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.76171875" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="29.375" customWidth="1"/>
+    <col min="5" max="5" width="29.3515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>177</v>
       </c>
@@ -2127,7 +2119,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.3">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -2143,12 +2135,14 @@
       <c r="E2" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="F2" s="19"/>
+      <c r="F2" t="s">
+        <v>172</v>
+      </c>
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
       <c r="I2" s="18"/>
     </row>
-    <row r="3" spans="1:9" ht="63" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.3">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -2164,12 +2158,14 @@
       <c r="E3" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="19"/>
+      <c r="F3" t="s">
+        <v>184</v>
+      </c>
       <c r="G3" s="19"/>
       <c r="H3" s="19"/>
       <c r="I3" s="18"/>
     </row>
-    <row r="4" spans="1:9" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.3">
       <c r="A4" s="18">
         <v>3</v>
       </c>
@@ -2185,12 +2181,14 @@
       <c r="E4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="19"/>
+      <c r="F4" t="s">
+        <v>179</v>
+      </c>
       <c r="G4" s="19"/>
       <c r="H4" s="19"/>
       <c r="I4" s="18"/>
     </row>
-    <row r="5" spans="1:9" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.3">
       <c r="A5" s="18">
         <v>4</v>
       </c>
@@ -2206,12 +2204,14 @@
       <c r="E5" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="19"/>
+      <c r="F5" t="s">
+        <v>191</v>
+      </c>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
       <c r="I5" s="18"/>
     </row>
-    <row r="6" spans="1:9" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.3">
       <c r="A6" s="18">
         <v>5</v>
       </c>
@@ -2227,12 +2227,14 @@
       <c r="E6" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="19"/>
+      <c r="F6" t="s">
+        <v>191</v>
+      </c>
       <c r="G6" s="19"/>
       <c r="H6" s="19"/>
       <c r="I6" s="18"/>
     </row>
-    <row r="7" spans="1:9" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.3">
       <c r="A7" s="18">
         <v>6</v>
       </c>
@@ -2248,12 +2250,14 @@
       <c r="E7" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="19"/>
+      <c r="F7" t="s">
+        <v>172</v>
+      </c>
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
       <c r="I7" s="18"/>
     </row>
-    <row r="8" spans="1:9" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.3">
       <c r="A8" s="18">
         <v>7</v>
       </c>
@@ -2269,12 +2273,14 @@
       <c r="E8" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="19"/>
+      <c r="F8" t="s">
+        <v>179</v>
+      </c>
       <c r="G8" s="19"/>
       <c r="H8" s="19"/>
       <c r="I8" s="18"/>
     </row>
-    <row r="9" spans="1:9" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.3">
       <c r="A9" s="18">
         <v>8</v>
       </c>
@@ -2290,12 +2296,14 @@
       <c r="E9" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="F9" s="19"/>
+      <c r="F9" t="s">
+        <v>184</v>
+      </c>
       <c r="G9" s="19"/>
       <c r="H9" s="19"/>
       <c r="I9" s="18"/>
     </row>
-    <row r="10" spans="1:9" ht="63" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="18"/>
       <c r="C10" s="18" t="s">
@@ -2312,7 +2320,7 @@
       <c r="H10" s="19"/>
       <c r="I10" s="18"/>
     </row>
-    <row r="11" spans="1:9" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
       <c r="C11" s="18" t="s">
@@ -2329,7 +2337,7 @@
       <c r="H11" s="19"/>
       <c r="I11" s="18"/>
     </row>
-    <row r="12" spans="1:9" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="18"/>
       <c r="C12" s="18" t="s">
@@ -2346,7 +2354,7 @@
       <c r="H12" s="19"/>
       <c r="I12" s="18"/>
     </row>
-    <row r="13" spans="1:9" ht="63" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="60" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
       <c r="C13" s="18" t="s">
@@ -2363,7 +2371,7 @@
       <c r="H13" s="19"/>
       <c r="I13" s="18"/>
     </row>
-    <row r="14" spans="1:9" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.3">
       <c r="A14" s="18"/>
       <c r="B14" s="18"/>
       <c r="C14" s="18" t="s">
@@ -2380,7 +2388,7 @@
       <c r="H14" s="19"/>
       <c r="I14" s="18"/>
     </row>
-    <row r="15" spans="1:9" ht="63" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.3">
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
       <c r="C15" s="18" t="s">
@@ -2397,7 +2405,7 @@
       <c r="H15" s="19"/>
       <c r="I15" s="18"/>
     </row>
-    <row r="16" spans="1:9" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
       <c r="B16" s="18"/>
       <c r="C16" s="18" t="s">
@@ -2414,7 +2422,7 @@
       <c r="H16" s="19"/>
       <c r="I16" s="18"/>
     </row>
-    <row r="17" spans="3:8" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:8" ht="60" x14ac:dyDescent="0.3">
       <c r="C17" s="18" t="s">
         <v>118</v>
       </c>
@@ -2428,7 +2436,7 @@
       <c r="G17" s="19"/>
       <c r="H17" s="19"/>
     </row>
-    <row r="18" spans="3:8" ht="110.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:8" ht="90" x14ac:dyDescent="0.3">
       <c r="C18" s="18" t="s">
         <v>119</v>
       </c>
@@ -2442,7 +2450,7 @@
       <c r="G18" s="19"/>
       <c r="H18" s="19"/>
     </row>
-    <row r="19" spans="3:8" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:8" ht="30" x14ac:dyDescent="0.3">
       <c r="C19" s="18" t="s">
         <v>120</v>
       </c>
@@ -2456,7 +2464,7 @@
       <c r="G19" s="19"/>
       <c r="H19" s="19"/>
     </row>
-    <row r="20" spans="3:8" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:8" ht="30" x14ac:dyDescent="0.3">
       <c r="C20" s="18" t="s">
         <v>121</v>
       </c>
@@ -2470,7 +2478,7 @@
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
     </row>
-    <row r="21" spans="3:8" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:8" ht="30" x14ac:dyDescent="0.3">
       <c r="C21" s="18" t="s">
         <v>123</v>
       </c>
@@ -2484,7 +2492,7 @@
       <c r="G21" s="19"/>
       <c r="H21" s="19"/>
     </row>
-    <row r="22" spans="3:8" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:8" ht="30" x14ac:dyDescent="0.3">
       <c r="C22" s="18" t="s">
         <v>124</v>
       </c>
@@ -2498,7 +2506,7 @@
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
     </row>
-    <row r="23" spans="3:8" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:8" ht="30" x14ac:dyDescent="0.3">
       <c r="C23" s="18" t="s">
         <v>125</v>
       </c>
@@ -2512,7 +2520,7 @@
       <c r="G23" s="19"/>
       <c r="H23" s="19"/>
     </row>
-    <row r="24" spans="3:8" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:8" ht="30" x14ac:dyDescent="0.3">
       <c r="C24" s="18" t="s">
         <v>126</v>
       </c>
@@ -2526,7 +2534,7 @@
       <c r="G24" s="19"/>
       <c r="H24" s="19"/>
     </row>
-    <row r="25" spans="3:8" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:8" ht="60" x14ac:dyDescent="0.3">
       <c r="C25" s="18" t="s">
         <v>130</v>
       </c>
@@ -2540,7 +2548,7 @@
       <c r="G25" s="19"/>
       <c r="H25" s="19"/>
     </row>
-    <row r="26" spans="3:8" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:8" ht="45" x14ac:dyDescent="0.3">
       <c r="C26" s="18" t="s">
         <v>131</v>
       </c>
@@ -2554,7 +2562,7 @@
       <c r="G26" s="19"/>
       <c r="H26" s="19"/>
     </row>
-    <row r="27" spans="3:8" ht="204.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:8" ht="195" x14ac:dyDescent="0.3">
       <c r="C27" s="18" t="s">
         <v>132</v>
       </c>
@@ -2568,7 +2576,7 @@
       <c r="G27" s="19"/>
       <c r="H27" s="19"/>
     </row>
-    <row r="28" spans="3:8" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:8" ht="30" x14ac:dyDescent="0.3">
       <c r="C28" s="18" t="s">
         <v>133</v>
       </c>
@@ -2582,7 +2590,7 @@
       <c r="G28" s="19"/>
       <c r="H28" s="19"/>
     </row>
-    <row r="29" spans="3:8" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:8" ht="45" x14ac:dyDescent="0.3">
       <c r="C29" s="18" t="s">
         <v>134</v>
       </c>
@@ -2596,7 +2604,7 @@
       <c r="G29" s="19"/>
       <c r="H29" s="19"/>
     </row>
-    <row r="30" spans="3:8" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:8" ht="30" x14ac:dyDescent="0.3">
       <c r="C30" s="18" t="s">
         <v>135</v>
       </c>
@@ -2610,7 +2618,7 @@
       <c r="G30" s="19"/>
       <c r="H30" s="19"/>
     </row>
-    <row r="31" spans="3:8" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:8" ht="30" x14ac:dyDescent="0.3">
       <c r="C31" s="18" t="s">
         <v>136</v>
       </c>
@@ -2624,7 +2632,7 @@
       <c r="G31" s="19"/>
       <c r="H31" s="19"/>
     </row>
-    <row r="32" spans="3:8" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:8" ht="45" x14ac:dyDescent="0.3">
       <c r="C32" s="18" t="s">
         <v>137</v>
       </c>
@@ -2638,7 +2646,7 @@
       <c r="G32" s="19"/>
       <c r="H32" s="19"/>
     </row>
-    <row r="33" spans="3:8" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:8" ht="30" x14ac:dyDescent="0.3">
       <c r="C33" s="18" t="s">
         <v>138</v>
       </c>
@@ -2653,7 +2661,7 @@
       <c r="H33" s="19"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1"/>
+  <autoFilter ref="A1:H1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2666,54 +2674,54 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="7"/>
-    <col min="2" max="2" width="9.375" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.25" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="9.3515625" customWidth="1"/>
+    <col min="3" max="3" width="15.87890625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.234375" customWidth="1"/>
+    <col min="5" max="5" width="6.87890625" customWidth="1"/>
+    <col min="6" max="6" width="12.3515625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>154</v>
       </c>
@@ -2736,7 +2744,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>155</v>
       </c>
@@ -2752,7 +2760,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>156</v>
       </c>
@@ -2777,7 +2785,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>157</v>
       </c>
@@ -2802,7 +2810,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>158</v>
       </c>
@@ -2827,7 +2835,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>159</v>
       </c>
@@ -2865,24 +2873,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="2"/>
-    <col min="2" max="2" width="16.75" customWidth="1"/>
-    <col min="3" max="3" width="12.375" customWidth="1"/>
-    <col min="4" max="4" width="7.125" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="16.76171875" customWidth="1"/>
+    <col min="3" max="3" width="12.3515625" customWidth="1"/>
+    <col min="4" max="4" width="7.1171875" customWidth="1"/>
+    <col min="5" max="5" width="6.87890625" customWidth="1"/>
+    <col min="6" max="6" width="12.3515625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2902,37 +2910,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
-        <v>40442</v>
+        <v>41676</v>
       </c>
       <c r="B2">
-        <v>36</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <v>40455</v>
-      </c>
-      <c r="B3">
-        <v>30</v>
-      </c>
-      <c r="C3">
-        <f>B2-B3</f>
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>250</v>
-      </c>
-      <c r="E3">
-        <v>120</v>
-      </c>
-      <c r="F3" s="9">
-        <f>(D3-D2)/E3*60</f>
-        <v>125.00000000000001</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2949,26 +2932,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.75" customWidth="1"/>
-    <col min="2" max="2" width="24.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.75" customWidth="1"/>
-    <col min="5" max="5" width="9.25" customWidth="1"/>
-    <col min="6" max="6" width="10.375" customWidth="1"/>
-    <col min="7" max="7" width="9.125" customWidth="1"/>
+    <col min="1" max="1" width="7.76171875" customWidth="1"/>
+    <col min="2" max="2" width="24.3515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.76171875" customWidth="1"/>
+    <col min="5" max="5" width="9.234375" customWidth="1"/>
+    <col min="6" max="6" width="10.3515625" customWidth="1"/>
+    <col min="7" max="7" width="9.1171875" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="11.25" style="6" customWidth="1"/>
+    <col min="9" max="9" width="11.234375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2997,7 +2978,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>128</v>
       </c>
@@ -3008,7 +2989,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>129</v>
       </c>
@@ -3025,7 +3006,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>122</v>
       </c>
@@ -3042,23 +3023,29 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>107</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>108</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>109</v>
       </c>
@@ -3069,7 +3056,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>113</v>
       </c>
@@ -3086,7 +3073,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>127</v>
       </c>
@@ -3103,21 +3090,21 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" s="5"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>26</v>
       </c>
@@ -3135,16 +3122,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3186,16 +3173,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3236,16 +3223,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3286,20 +3273,18 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C33" sqref="A2:C33"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1171875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.3515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>106</v>
       </c>
@@ -3310,7 +3295,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -3321,7 +3306,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -3332,7 +3317,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -3343,7 +3328,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -3354,7 +3339,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>111</v>
       </c>
@@ -3365,7 +3350,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -3376,7 +3361,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>113</v>
       </c>
@@ -3387,7 +3372,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -3398,7 +3383,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>115</v>
       </c>
@@ -3409,7 +3394,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>116</v>
       </c>
@@ -3420,7 +3405,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>117</v>
       </c>
@@ -3431,7 +3416,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>118</v>
       </c>
@@ -3442,7 +3427,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>119</v>
       </c>
@@ -3453,7 +3438,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>120</v>
       </c>
@@ -3464,7 +3449,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>121</v>
       </c>
@@ -3475,7 +3460,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>122</v>
       </c>
@@ -3486,7 +3471,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>123</v>
       </c>
@@ -3497,7 +3482,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>124</v>
       </c>
@@ -3508,7 +3493,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>125</v>
       </c>
@@ -3519,7 +3504,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>126</v>
       </c>
@@ -3530,7 +3515,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>127</v>
       </c>
@@ -3541,7 +3526,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>128</v>
       </c>
@@ -3552,7 +3537,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>129</v>
       </c>
@@ -3563,7 +3548,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>130</v>
       </c>
@@ -3574,7 +3559,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>131</v>
       </c>
@@ -3585,7 +3570,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="126" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>132</v>
       </c>
@@ -3596,7 +3581,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>133</v>
       </c>
@@ -3607,7 +3592,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>134</v>
       </c>
@@ -3618,7 +3603,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>135</v>
       </c>
@@ -3629,7 +3614,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>136</v>
       </c>
@@ -3640,7 +3625,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>137</v>
       </c>
@@ -3651,7 +3636,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>138</v>
       </c>
@@ -3662,7 +3647,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>139</v>
       </c>
@@ -3673,7 +3658,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>140</v>
       </c>
@@ -3684,7 +3669,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>141</v>
       </c>
@@ -3695,7 +3680,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>142</v>
       </c>
@@ -3706,7 +3691,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>143</v>
       </c>
@@ -3717,7 +3702,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>144</v>
       </c>
@@ -3728,7 +3713,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>145</v>
       </c>
@@ -3739,7 +3724,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>146</v>
       </c>
@@ -3750,7 +3735,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>147</v>
       </c>
@@ -3761,7 +3746,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>148</v>
       </c>

</xml_diff>

<commit_message>
Adding story code and time estimations
</commit_message>
<xml_diff>
--- a/TeamEstherKarelKeithTroyReport.xlsx
+++ b/TeamEstherKarelKeithTroyReport.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klros\Google Drive\Keith\Stevens Institute of Technology\SSW-555-WS\Projects\cs555\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KLahmy\Documents\stevens\CS-555\project\GIT\stevens_cs555\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" tabRatio="627" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9468" tabRatio="627" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -25,11 +25,8 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backlog!$A$1:$H$1</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -649,7 +646,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -887,7 +884,7 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="68" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
+    <cellStyle name="Normal 2" xfId="68"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -903,7 +900,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -974,7 +971,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8005-41C3-A2A6-994BE20B6C54}"/>
             </c:ext>
@@ -990,11 +987,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2078309640"/>
-        <c:axId val="2078306552"/>
+        <c:axId val="182988040"/>
+        <c:axId val="182995584"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2078309640"/>
+        <c:axId val="182988040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1004,14 +1001,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2078306552"/>
+        <c:crossAx val="182995584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2078306552"/>
+        <c:axId val="182995584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1022,7 +1019,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2078309640"/>
+        <c:crossAx val="182988040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1040,7 +1037,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1087,7 +1084,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5A9F-42BD-9352-89747C7C9AC0}"/>
             </c:ext>
@@ -1103,11 +1100,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2141804184"/>
-        <c:axId val="2141807272"/>
+        <c:axId val="184204616"/>
+        <c:axId val="183298384"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2141804184"/>
+        <c:axId val="184204616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1117,14 +1114,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2141807272"/>
+        <c:crossAx val="183298384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2141807272"/>
+        <c:axId val="183298384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1135,7 +1132,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2141804184"/>
+        <c:crossAx val="184204616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1172,7 +1169,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1210,7 +1207,7 @@
         <xdr:cNvPr id="3" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1285,7 +1282,7 @@
         <xdr:cNvPr id="4" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1350,7 +1347,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1419,7 +1416,7 @@
         <xdr:cNvPr id="6" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1489,7 +1486,7 @@
         <xdr:cNvPr id="7" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1558,7 +1555,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1628,7 +1625,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1968,20 +1965,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.87890625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.3515625" customWidth="1"/>
-    <col min="3" max="3" width="10.87890625" customWidth="1"/>
-    <col min="4" max="4" width="20.3515625" customWidth="1"/>
+    <col min="1" max="1" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.36328125" customWidth="1"/>
+    <col min="3" max="3" width="10.90625" customWidth="1"/>
+    <col min="4" max="4" width="20.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -1995,7 +1992,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>172</v>
       </c>
@@ -2009,7 +2006,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>179</v>
       </c>
@@ -2023,7 +2020,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>184</v>
       </c>
@@ -2037,7 +2034,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>191</v>
       </c>
@@ -2051,7 +2048,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>192</v>
       </c>
@@ -2065,7 +2062,7 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D9" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2078,19 +2075,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.76171875" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="29.3515625" customWidth="1"/>
+    <col min="5" max="5" width="29.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>177</v>
       </c>
@@ -2119,7 +2116,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -2142,7 +2139,7 @@
       <c r="H2" s="19"/>
       <c r="I2" s="18"/>
     </row>
-    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -2165,7 +2162,7 @@
       <c r="H3" s="19"/>
       <c r="I3" s="18"/>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="18">
         <v>3</v>
       </c>
@@ -2188,7 +2185,7 @@
       <c r="H4" s="19"/>
       <c r="I4" s="18"/>
     </row>
-    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A5" s="18">
         <v>4</v>
       </c>
@@ -2211,7 +2208,7 @@
       <c r="H5" s="19"/>
       <c r="I5" s="18"/>
     </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="18">
         <v>5</v>
       </c>
@@ -2234,7 +2231,7 @@
       <c r="H6" s="19"/>
       <c r="I6" s="18"/>
     </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" s="18">
         <v>6</v>
       </c>
@@ -2257,7 +2254,7 @@
       <c r="H7" s="19"/>
       <c r="I7" s="18"/>
     </row>
-    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.2">
       <c r="A8" s="18">
         <v>7</v>
       </c>
@@ -2280,7 +2277,7 @@
       <c r="H8" s="19"/>
       <c r="I8" s="18"/>
     </row>
-    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A9" s="18">
         <v>8</v>
       </c>
@@ -2303,7 +2300,7 @@
       <c r="H9" s="19"/>
       <c r="I9" s="18"/>
     </row>
-    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A10" s="18"/>
       <c r="B10" s="18"/>
       <c r="C10" s="18" t="s">
@@ -2320,7 +2317,7 @@
       <c r="H10" s="19"/>
       <c r="I10" s="18"/>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
       <c r="C11" s="18" t="s">
@@ -2337,7 +2334,7 @@
       <c r="H11" s="19"/>
       <c r="I11" s="18"/>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="18"/>
       <c r="B12" s="18"/>
       <c r="C12" s="18" t="s">
@@ -2354,7 +2351,7 @@
       <c r="H12" s="19"/>
       <c r="I12" s="18"/>
     </row>
-    <row r="13" spans="1:9" ht="60" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
       <c r="C13" s="18" t="s">
@@ -2371,7 +2368,7 @@
       <c r="H13" s="19"/>
       <c r="I13" s="18"/>
     </row>
-    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" s="18"/>
       <c r="B14" s="18"/>
       <c r="C14" s="18" t="s">
@@ -2388,7 +2385,7 @@
       <c r="H14" s="19"/>
       <c r="I14" s="18"/>
     </row>
-    <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
       <c r="C15" s="18" t="s">
@@ -2405,7 +2402,7 @@
       <c r="H15" s="19"/>
       <c r="I15" s="18"/>
     </row>
-    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" s="18"/>
       <c r="B16" s="18"/>
       <c r="C16" s="18" t="s">
@@ -2422,7 +2419,7 @@
       <c r="H16" s="19"/>
       <c r="I16" s="18"/>
     </row>
-    <row r="17" spans="3:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:8" ht="60" x14ac:dyDescent="0.2">
       <c r="C17" s="18" t="s">
         <v>118</v>
       </c>
@@ -2436,7 +2433,7 @@
       <c r="G17" s="19"/>
       <c r="H17" s="19"/>
     </row>
-    <row r="18" spans="3:8" ht="90" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:8" ht="90" x14ac:dyDescent="0.2">
       <c r="C18" s="18" t="s">
         <v>119</v>
       </c>
@@ -2450,7 +2447,7 @@
       <c r="G18" s="19"/>
       <c r="H18" s="19"/>
     </row>
-    <row r="19" spans="3:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:8" ht="30" x14ac:dyDescent="0.2">
       <c r="C19" s="18" t="s">
         <v>120</v>
       </c>
@@ -2464,7 +2461,7 @@
       <c r="G19" s="19"/>
       <c r="H19" s="19"/>
     </row>
-    <row r="20" spans="3:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:8" ht="30" x14ac:dyDescent="0.2">
       <c r="C20" s="18" t="s">
         <v>121</v>
       </c>
@@ -2478,7 +2475,7 @@
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
     </row>
-    <row r="21" spans="3:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:8" ht="30" x14ac:dyDescent="0.2">
       <c r="C21" s="18" t="s">
         <v>123</v>
       </c>
@@ -2492,7 +2489,7 @@
       <c r="G21" s="19"/>
       <c r="H21" s="19"/>
     </row>
-    <row r="22" spans="3:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:8" ht="30" x14ac:dyDescent="0.2">
       <c r="C22" s="18" t="s">
         <v>124</v>
       </c>
@@ -2506,7 +2503,7 @@
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
     </row>
-    <row r="23" spans="3:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:8" ht="30" x14ac:dyDescent="0.2">
       <c r="C23" s="18" t="s">
         <v>125</v>
       </c>
@@ -2520,7 +2517,7 @@
       <c r="G23" s="19"/>
       <c r="H23" s="19"/>
     </row>
-    <row r="24" spans="3:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:8" ht="30" x14ac:dyDescent="0.2">
       <c r="C24" s="18" t="s">
         <v>126</v>
       </c>
@@ -2534,7 +2531,7 @@
       <c r="G24" s="19"/>
       <c r="H24" s="19"/>
     </row>
-    <row r="25" spans="3:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:8" ht="60" x14ac:dyDescent="0.2">
       <c r="C25" s="18" t="s">
         <v>130</v>
       </c>
@@ -2548,7 +2545,7 @@
       <c r="G25" s="19"/>
       <c r="H25" s="19"/>
     </row>
-    <row r="26" spans="3:8" ht="45" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:8" ht="45" x14ac:dyDescent="0.2">
       <c r="C26" s="18" t="s">
         <v>131</v>
       </c>
@@ -2562,7 +2559,7 @@
       <c r="G26" s="19"/>
       <c r="H26" s="19"/>
     </row>
-    <row r="27" spans="3:8" ht="195" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:8" ht="180" x14ac:dyDescent="0.2">
       <c r="C27" s="18" t="s">
         <v>132</v>
       </c>
@@ -2576,7 +2573,7 @@
       <c r="G27" s="19"/>
       <c r="H27" s="19"/>
     </row>
-    <row r="28" spans="3:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:8" ht="30" x14ac:dyDescent="0.2">
       <c r="C28" s="18" t="s">
         <v>133</v>
       </c>
@@ -2590,7 +2587,7 @@
       <c r="G28" s="19"/>
       <c r="H28" s="19"/>
     </row>
-    <row r="29" spans="3:8" ht="45" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:8" ht="45" x14ac:dyDescent="0.2">
       <c r="C29" s="18" t="s">
         <v>134</v>
       </c>
@@ -2604,7 +2601,7 @@
       <c r="G29" s="19"/>
       <c r="H29" s="19"/>
     </row>
-    <row r="30" spans="3:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:8" ht="30" x14ac:dyDescent="0.2">
       <c r="C30" s="18" t="s">
         <v>135</v>
       </c>
@@ -2618,7 +2615,7 @@
       <c r="G30" s="19"/>
       <c r="H30" s="19"/>
     </row>
-    <row r="31" spans="3:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:8" ht="30" x14ac:dyDescent="0.2">
       <c r="C31" s="18" t="s">
         <v>136</v>
       </c>
@@ -2632,7 +2629,7 @@
       <c r="G31" s="19"/>
       <c r="H31" s="19"/>
     </row>
-    <row r="32" spans="3:8" ht="45" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:8" ht="45" x14ac:dyDescent="0.2">
       <c r="C32" s="18" t="s">
         <v>137</v>
       </c>
@@ -2646,7 +2643,7 @@
       <c r="G32" s="19"/>
       <c r="H32" s="19"/>
     </row>
-    <row r="33" spans="3:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:8" ht="30" x14ac:dyDescent="0.2">
       <c r="C33" s="18" t="s">
         <v>138</v>
       </c>
@@ -2661,7 +2658,7 @@
       <c r="H33" s="19"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:H1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2674,54 +2671,54 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="7"/>
-    <col min="2" max="2" width="9.3515625" customWidth="1"/>
-    <col min="3" max="3" width="15.87890625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.234375" customWidth="1"/>
-    <col min="5" max="5" width="6.87890625" customWidth="1"/>
-    <col min="6" max="6" width="12.3515625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="9.36328125" customWidth="1"/>
+    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" customWidth="1"/>
+    <col min="6" max="6" width="12.36328125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>154</v>
       </c>
@@ -2744,7 +2741,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>155</v>
       </c>
@@ -2760,7 +2757,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>156</v>
       </c>
@@ -2785,7 +2782,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>157</v>
       </c>
@@ -2810,7 +2807,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>158</v>
       </c>
@@ -2835,7 +2832,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>159</v>
       </c>
@@ -2873,24 +2870,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="2"/>
-    <col min="2" max="2" width="16.76171875" customWidth="1"/>
-    <col min="3" max="3" width="12.3515625" customWidth="1"/>
-    <col min="4" max="4" width="7.1171875" customWidth="1"/>
-    <col min="5" max="5" width="6.87890625" customWidth="1"/>
-    <col min="6" max="6" width="12.3515625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" customWidth="1"/>
+    <col min="3" max="3" width="12.36328125" customWidth="1"/>
+    <col min="4" max="4" width="7.08984375" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" customWidth="1"/>
+    <col min="6" max="6" width="12.36328125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2910,7 +2907,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>41676</v>
       </c>
@@ -2932,24 +2929,26 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.76171875" customWidth="1"/>
-    <col min="2" max="2" width="24.3515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.76171875" customWidth="1"/>
-    <col min="5" max="5" width="9.234375" customWidth="1"/>
-    <col min="6" max="6" width="10.3515625" customWidth="1"/>
-    <col min="7" max="7" width="9.1171875" customWidth="1"/>
+    <col min="1" max="1" width="7.7265625" customWidth="1"/>
+    <col min="2" max="2" width="24.36328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7265625" customWidth="1"/>
+    <col min="5" max="5" width="9.26953125" customWidth="1"/>
+    <col min="6" max="6" width="10.36328125" customWidth="1"/>
+    <col min="7" max="7" width="9.08984375" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="11.234375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="11.26953125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2978,7 +2977,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>128</v>
       </c>
@@ -2989,7 +2988,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
         <v>129</v>
       </c>
@@ -3006,7 +3005,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>122</v>
       </c>
@@ -3023,7 +3022,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
         <v>107</v>
       </c>
@@ -3033,8 +3032,14 @@
       <c r="C5" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
         <v>108</v>
       </c>
@@ -3044,8 +3049,14 @@
       <c r="C6" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
         <v>109</v>
       </c>
@@ -3056,7 +3067,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
         <v>113</v>
       </c>
@@ -3073,7 +3084,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
         <v>127</v>
       </c>
@@ -3090,21 +3101,21 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="5"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
         <v>26</v>
       </c>
@@ -3122,16 +3133,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3173,16 +3184,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3223,16 +3234,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3273,18 +3284,18 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.1171875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.3515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.36328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>106</v>
       </c>
@@ -3295,7 +3306,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -3306,7 +3317,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -3317,7 +3328,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -3328,7 +3339,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -3339,7 +3350,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>111</v>
       </c>
@@ -3350,7 +3361,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -3361,7 +3372,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>113</v>
       </c>
@@ -3372,7 +3383,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -3383,7 +3394,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>115</v>
       </c>
@@ -3394,7 +3405,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>116</v>
       </c>
@@ -3405,7 +3416,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>117</v>
       </c>
@@ -3416,7 +3427,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>118</v>
       </c>
@@ -3427,7 +3438,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>119</v>
       </c>
@@ -3438,7 +3449,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>120</v>
       </c>
@@ -3449,7 +3460,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>121</v>
       </c>
@@ -3460,7 +3471,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>122</v>
       </c>
@@ -3471,7 +3482,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>123</v>
       </c>
@@ -3482,7 +3493,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>124</v>
       </c>
@@ -3493,7 +3504,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>125</v>
       </c>
@@ -3504,7 +3515,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>126</v>
       </c>
@@ -3515,7 +3526,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>127</v>
       </c>
@@ -3526,7 +3537,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>128</v>
       </c>
@@ -3537,7 +3548,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>129</v>
       </c>
@@ -3548,7 +3559,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>130</v>
       </c>
@@ -3559,7 +3570,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>131</v>
       </c>
@@ -3570,7 +3581,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>132</v>
       </c>
@@ -3581,7 +3592,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>133</v>
       </c>
@@ -3592,7 +3603,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>134</v>
       </c>
@@ -3603,7 +3614,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>135</v>
       </c>
@@ -3614,7 +3625,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>136</v>
       </c>
@@ -3625,7 +3636,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>137</v>
       </c>
@@ -3636,7 +3647,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>138</v>
       </c>
@@ -3647,7 +3658,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>139</v>
       </c>
@@ -3658,7 +3669,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>140</v>
       </c>
@@ -3669,7 +3680,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>141</v>
       </c>
@@ -3680,7 +3691,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>142</v>
       </c>
@@ -3691,7 +3702,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>143</v>
       </c>
@@ -3702,7 +3713,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>144</v>
       </c>
@@ -3713,7 +3724,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>145</v>
       </c>
@@ -3724,7 +3735,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>146</v>
       </c>
@@ -3735,7 +3746,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>147</v>
       </c>
@@ -3746,7 +3757,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>148</v>
       </c>

</xml_diff>

<commit_message>
updated projected points for sprint 1
</commit_message>
<xml_diff>
--- a/TeamEstherKarelKeithTroyReport.xlsx
+++ b/TeamEstherKarelKeithTroyReport.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28705"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KLahmy\Documents\stevens\CS-555\project\GIT\stevens_cs555\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9468" tabRatio="627" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="16420" tabRatio="627" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -25,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backlog!$A$1:$H$1</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -35,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="194">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -926,22 +921,22 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41065</c:v>
+                  <c:v>41065.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41078</c:v>
+                  <c:v>41078.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41092</c:v>
+                  <c:v>41092.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41106</c:v>
+                  <c:v>41106.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41120</c:v>
+                  <c:v>41120.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -953,19 +948,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -987,28 +982,28 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="182988040"/>
-        <c:axId val="182995584"/>
+        <c:axId val="-2139013128"/>
+        <c:axId val="-2139017864"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="182988040"/>
+        <c:axId val="-2139013128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182995584"/>
+        <c:crossAx val="-2139017864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="182995584"/>
+        <c:axId val="-2139017864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1019,7 +1014,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182988040"/>
+        <c:crossAx val="-2139013128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1030,7 +1025,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1061,24 +1056,24 @@
           <c:order val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Burndown!$A$2:$A$7</c:f>
+              <c:f>Burndown!$B$2:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41676</c:v>
+                  <c:v>41676.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Burndown!$B$2:$B$7</c:f>
+              <c:f>Burndown!$C$2:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1100,11 +1095,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="184204616"/>
-        <c:axId val="183298384"/>
+        <c:axId val="-2136333176"/>
+        <c:axId val="-2136330104"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="184204616"/>
+        <c:axId val="-2136333176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1114,14 +1109,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="183298384"/>
+        <c:crossAx val="-2136330104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="183298384"/>
+        <c:axId val="-2136330104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1132,7 +1127,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="184204616"/>
+        <c:crossAx val="-2136333176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1143,7 +1138,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1169,7 +1164,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1207,7 +1202,7 @@
         <xdr:cNvPr id="3" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1282,7 +1277,7 @@
         <xdr:cNvPr id="4" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1347,7 +1342,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1416,7 +1411,7 @@
         <xdr:cNvPr id="6" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1486,7 +1481,7 @@
         <xdr:cNvPr id="7" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1555,7 +1550,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1610,22 +1605,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>948267</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>160867</xdr:rowOff>
+      <xdr:colOff>376767</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>84667</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>397934</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>25401</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>563034</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1968,17 +1963,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.36328125" customWidth="1"/>
-    <col min="3" max="3" width="10.90625" customWidth="1"/>
-    <col min="4" max="4" width="20.36328125" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -1992,7 +1987,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>172</v>
       </c>
@@ -2006,7 +2001,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>179</v>
       </c>
@@ -2020,7 +2015,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>184</v>
       </c>
@@ -2034,7 +2029,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>191</v>
       </c>
@@ -2048,7 +2043,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="C9" t="s">
         <v>192</v>
       </c>
@@ -2078,16 +2073,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="5" max="5" width="29.36328125" customWidth="1"/>
+    <col min="5" max="5" width="29.42578125" customWidth="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="17" t="s">
         <v>177</v>
       </c>
@@ -2116,7 +2113,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="30">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -2139,7 +2136,7 @@
       <c r="H2" s="19"/>
       <c r="I2" s="18"/>
     </row>
-    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="45">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -2162,7 +2159,7 @@
       <c r="H3" s="19"/>
       <c r="I3" s="18"/>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="30">
       <c r="A4" s="18">
         <v>3</v>
       </c>
@@ -2185,7 +2182,7 @@
       <c r="H4" s="19"/>
       <c r="I4" s="18"/>
     </row>
-    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="45">
       <c r="A5" s="18">
         <v>4</v>
       </c>
@@ -2208,7 +2205,7 @@
       <c r="H5" s="19"/>
       <c r="I5" s="18"/>
     </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="30">
       <c r="A6" s="18">
         <v>5</v>
       </c>
@@ -2231,7 +2228,7 @@
       <c r="H6" s="19"/>
       <c r="I6" s="18"/>
     </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="30">
       <c r="A7" s="18">
         <v>6</v>
       </c>
@@ -2254,7 +2251,7 @@
       <c r="H7" s="19"/>
       <c r="I7" s="18"/>
     </row>
-    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="60">
       <c r="A8" s="18">
         <v>7</v>
       </c>
@@ -2277,7 +2274,7 @@
       <c r="H8" s="19"/>
       <c r="I8" s="18"/>
     </row>
-    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="30">
       <c r="A9" s="18">
         <v>8</v>
       </c>
@@ -2300,7 +2297,7 @@
       <c r="H9" s="19"/>
       <c r="I9" s="18"/>
     </row>
-    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="45">
       <c r="A10" s="18"/>
       <c r="B10" s="18"/>
       <c r="C10" s="18" t="s">
@@ -2317,7 +2314,7 @@
       <c r="H10" s="19"/>
       <c r="I10" s="18"/>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="30">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
       <c r="C11" s="18" t="s">
@@ -2334,7 +2331,7 @@
       <c r="H11" s="19"/>
       <c r="I11" s="18"/>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="30">
       <c r="A12" s="18"/>
       <c r="B12" s="18"/>
       <c r="C12" s="18" t="s">
@@ -2351,7 +2348,7 @@
       <c r="H12" s="19"/>
       <c r="I12" s="18"/>
     </row>
-    <row r="13" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="45">
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
       <c r="C13" s="18" t="s">
@@ -2368,7 +2365,7 @@
       <c r="H13" s="19"/>
       <c r="I13" s="18"/>
     </row>
-    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="45">
       <c r="A14" s="18"/>
       <c r="B14" s="18"/>
       <c r="C14" s="18" t="s">
@@ -2385,7 +2382,7 @@
       <c r="H14" s="19"/>
       <c r="I14" s="18"/>
     </row>
-    <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="45">
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
       <c r="C15" s="18" t="s">
@@ -2402,7 +2399,7 @@
       <c r="H15" s="19"/>
       <c r="I15" s="18"/>
     </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="30">
       <c r="A16" s="18"/>
       <c r="B16" s="18"/>
       <c r="C16" s="18" t="s">
@@ -2419,7 +2416,7 @@
       <c r="H16" s="19"/>
       <c r="I16" s="18"/>
     </row>
-    <row r="17" spans="3:8" ht="60" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:8" ht="60">
       <c r="C17" s="18" t="s">
         <v>118</v>
       </c>
@@ -2433,7 +2430,7 @@
       <c r="G17" s="19"/>
       <c r="H17" s="19"/>
     </row>
-    <row r="18" spans="3:8" ht="90" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:8" ht="90">
       <c r="C18" s="18" t="s">
         <v>119</v>
       </c>
@@ -2447,7 +2444,7 @@
       <c r="G18" s="19"/>
       <c r="H18" s="19"/>
     </row>
-    <row r="19" spans="3:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:8" ht="30">
       <c r="C19" s="18" t="s">
         <v>120</v>
       </c>
@@ -2461,7 +2458,7 @@
       <c r="G19" s="19"/>
       <c r="H19" s="19"/>
     </row>
-    <row r="20" spans="3:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:8" ht="30">
       <c r="C20" s="18" t="s">
         <v>121</v>
       </c>
@@ -2475,7 +2472,7 @@
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
     </row>
-    <row r="21" spans="3:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:8" ht="30">
       <c r="C21" s="18" t="s">
         <v>123</v>
       </c>
@@ -2489,7 +2486,7 @@
       <c r="G21" s="19"/>
       <c r="H21" s="19"/>
     </row>
-    <row r="22" spans="3:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:8" ht="30">
       <c r="C22" s="18" t="s">
         <v>124</v>
       </c>
@@ -2503,7 +2500,7 @@
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
     </row>
-    <row r="23" spans="3:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:8" ht="30">
       <c r="C23" s="18" t="s">
         <v>125</v>
       </c>
@@ -2517,7 +2514,7 @@
       <c r="G23" s="19"/>
       <c r="H23" s="19"/>
     </row>
-    <row r="24" spans="3:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:8" ht="30">
       <c r="C24" s="18" t="s">
         <v>126</v>
       </c>
@@ -2531,7 +2528,7 @@
       <c r="G24" s="19"/>
       <c r="H24" s="19"/>
     </row>
-    <row r="25" spans="3:8" ht="60" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:8" ht="60">
       <c r="C25" s="18" t="s">
         <v>130</v>
       </c>
@@ -2545,7 +2542,7 @@
       <c r="G25" s="19"/>
       <c r="H25" s="19"/>
     </row>
-    <row r="26" spans="3:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:8" ht="45">
       <c r="C26" s="18" t="s">
         <v>131</v>
       </c>
@@ -2559,7 +2556,7 @@
       <c r="G26" s="19"/>
       <c r="H26" s="19"/>
     </row>
-    <row r="27" spans="3:8" ht="180" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:8" ht="165">
       <c r="C27" s="18" t="s">
         <v>132</v>
       </c>
@@ -2573,7 +2570,7 @@
       <c r="G27" s="19"/>
       <c r="H27" s="19"/>
     </row>
-    <row r="28" spans="3:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:8" ht="30">
       <c r="C28" s="18" t="s">
         <v>133</v>
       </c>
@@ -2587,7 +2584,7 @@
       <c r="G28" s="19"/>
       <c r="H28" s="19"/>
     </row>
-    <row r="29" spans="3:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:8" ht="45">
       <c r="C29" s="18" t="s">
         <v>134</v>
       </c>
@@ -2601,7 +2598,7 @@
       <c r="G29" s="19"/>
       <c r="H29" s="19"/>
     </row>
-    <row r="30" spans="3:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:8" ht="30">
       <c r="C30" s="18" t="s">
         <v>135</v>
       </c>
@@ -2615,7 +2612,7 @@
       <c r="G30" s="19"/>
       <c r="H30" s="19"/>
     </row>
-    <row r="31" spans="3:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:8" ht="30">
       <c r="C31" s="18" t="s">
         <v>136</v>
       </c>
@@ -2629,7 +2626,7 @@
       <c r="G31" s="19"/>
       <c r="H31" s="19"/>
     </row>
-    <row r="32" spans="3:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:8" ht="45">
       <c r="C32" s="18" t="s">
         <v>137</v>
       </c>
@@ -2643,7 +2640,7 @@
       <c r="G32" s="19"/>
       <c r="H32" s="19"/>
     </row>
-    <row r="33" spans="3:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:8" ht="30">
       <c r="C33" s="18" t="s">
         <v>138</v>
       </c>
@@ -2674,51 +2671,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11" style="7"/>
-    <col min="2" max="2" width="9.36328125" customWidth="1"/>
-    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.26953125" customWidth="1"/>
-    <col min="5" max="5" width="6.90625" customWidth="1"/>
-    <col min="6" max="6" width="12.36328125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" s="7" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="7" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="7" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" s="7" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="4" customFormat="1">
       <c r="A14" s="4" t="s">
         <v>154</v>
       </c>
@@ -2741,7 +2738,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>155</v>
       </c>
@@ -2757,7 +2754,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>156</v>
       </c>
@@ -2782,7 +2779,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" s="7" t="s">
         <v>157</v>
       </c>
@@ -2807,7 +2804,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" s="7" t="s">
         <v>158</v>
       </c>
@@ -2832,7 +2829,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" s="7" t="s">
         <v>159</v>
       </c>
@@ -2871,47 +2868,53 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11" style="2"/>
-    <col min="2" max="2" width="16.7265625" customWidth="1"/>
-    <col min="3" max="3" width="12.36328125" customWidth="1"/>
-    <col min="4" max="4" width="7.08984375" customWidth="1"/>
-    <col min="5" max="5" width="6.90625" customWidth="1"/>
-    <col min="6" max="6" width="12.36328125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="11" style="2"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" s="2">
         <v>41676</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>32</v>
       </c>
     </row>
@@ -2932,23 +2935,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.7265625" customWidth="1"/>
-    <col min="2" max="2" width="24.36328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7265625" customWidth="1"/>
-    <col min="5" max="5" width="9.26953125" customWidth="1"/>
-    <col min="6" max="6" width="10.36328125" customWidth="1"/>
-    <col min="7" max="7" width="9.08984375" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="11.26953125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2977,7 +2980,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="18" t="s">
         <v>128</v>
       </c>
@@ -2987,8 +2990,14 @@
       <c r="C2" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="18" t="s">
         <v>129</v>
       </c>
@@ -3005,7 +3014,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="18" t="s">
         <v>122</v>
       </c>
@@ -3022,7 +3031,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="18" t="s">
         <v>107</v>
       </c>
@@ -3039,7 +3048,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="18" t="s">
         <v>108</v>
       </c>
@@ -3056,7 +3065,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="18" t="s">
         <v>109</v>
       </c>
@@ -3066,8 +3075,14 @@
       <c r="C7" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="18" t="s">
         <v>113</v>
       </c>
@@ -3084,7 +3099,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" s="18" t="s">
         <v>127</v>
       </c>
@@ -3101,21 +3116,21 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="B14" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="B15" s="5"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="B16" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2">
       <c r="B20" s="5" t="s">
         <v>26</v>
       </c>
@@ -3136,13 +3151,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3187,13 +3202,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3237,13 +3252,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3287,15 +3302,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="28.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.36328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>106</v>
       </c>
@@ -3306,7 +3321,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="30">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -3317,7 +3332,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="15">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -3328,7 +3343,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="15">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -3339,7 +3354,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="30">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -3350,7 +3365,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="15">
       <c r="A6" t="s">
         <v>111</v>
       </c>
@@ -3361,7 +3376,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="15">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -3372,7 +3387,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="45">
       <c r="A8" t="s">
         <v>113</v>
       </c>
@@ -3383,7 +3398,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="30">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -3394,7 +3409,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="30">
       <c r="A10" t="s">
         <v>115</v>
       </c>
@@ -3405,7 +3420,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="30">
       <c r="A11" t="s">
         <v>116</v>
       </c>
@@ -3416,7 +3431,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="15">
       <c r="A12" t="s">
         <v>117</v>
       </c>
@@ -3427,7 +3442,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="30">
       <c r="A13" t="s">
         <v>118</v>
       </c>
@@ -3438,7 +3453,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="45">
       <c r="A14" t="s">
         <v>119</v>
       </c>
@@ -3449,7 +3464,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="15">
       <c r="A15" t="s">
         <v>120</v>
       </c>
@@ -3460,7 +3475,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="15">
       <c r="A16" t="s">
         <v>121</v>
       </c>
@@ -3471,7 +3486,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="15">
       <c r="A17" t="s">
         <v>122</v>
       </c>
@@ -3482,7 +3497,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="15">
       <c r="A18" t="s">
         <v>123</v>
       </c>
@@ -3493,7 +3508,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15">
       <c r="A19" t="s">
         <v>124</v>
       </c>
@@ -3504,7 +3519,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15">
       <c r="A20" t="s">
         <v>125</v>
       </c>
@@ -3515,7 +3530,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="15">
       <c r="A21" t="s">
         <v>126</v>
       </c>
@@ -3526,7 +3541,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="30">
       <c r="A22" t="s">
         <v>127</v>
       </c>
@@ -3537,7 +3552,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="30">
       <c r="A23" t="s">
         <v>128</v>
       </c>
@@ -3548,7 +3563,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="30">
       <c r="A24" t="s">
         <v>129</v>
       </c>
@@ -3559,7 +3574,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="30">
       <c r="A25" t="s">
         <v>130</v>
       </c>
@@ -3570,7 +3585,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="30">
       <c r="A26" t="s">
         <v>131</v>
       </c>
@@ -3581,7 +3596,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="90">
       <c r="A27" t="s">
         <v>132</v>
       </c>
@@ -3592,7 +3607,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="15">
       <c r="A28" t="s">
         <v>133</v>
       </c>
@@ -3603,7 +3618,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="30">
       <c r="A29" t="s">
         <v>134</v>
       </c>
@@ -3614,7 +3629,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="15">
       <c r="A30" t="s">
         <v>135</v>
       </c>
@@ -3625,7 +3640,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="15">
       <c r="A31" t="s">
         <v>136</v>
       </c>
@@ -3636,7 +3651,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="30">
       <c r="A32" t="s">
         <v>137</v>
       </c>
@@ -3647,7 +3662,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="15">
       <c r="A33" t="s">
         <v>138</v>
       </c>
@@ -3658,7 +3673,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="30">
       <c r="A34" t="s">
         <v>139</v>
       </c>
@@ -3669,7 +3684,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="30">
       <c r="A35" t="s">
         <v>140</v>
       </c>
@@ -3680,7 +3695,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="30">
       <c r="A36" t="s">
         <v>141</v>
       </c>
@@ -3691,7 +3706,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="15">
       <c r="A37" t="s">
         <v>142</v>
       </c>
@@ -3702,7 +3717,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="30">
       <c r="A38" t="s">
         <v>143</v>
       </c>
@@ -3713,7 +3728,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="30">
       <c r="A39" t="s">
         <v>144</v>
       </c>
@@ -3724,7 +3739,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="30">
       <c r="A40" t="s">
         <v>145</v>
       </c>
@@ -3735,7 +3750,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="30">
       <c r="A41" t="s">
         <v>146</v>
       </c>
@@ -3746,7 +3761,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="15">
       <c r="A42" t="s">
         <v>147</v>
       </c>
@@ -3757,7 +3772,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="30">
       <c r="A43" t="s">
         <v>148</v>
       </c>

</xml_diff>

<commit_message>
Added code for stories 01 02 Update report
</commit_message>
<xml_diff>
--- a/TeamEstherKarelKeithTroyReport.xlsx
+++ b/TeamEstherKarelKeithTroyReport.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KLahmy\Documents\stevens\CS-555\project\GIT\stevens_cs555\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="16420" tabRatio="627" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="-24" windowWidth="28800" windowHeight="16416" tabRatio="627" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -21,7 +26,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backlog!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sprint1!$A$1:$I$1</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="194">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -634,6 +639,9 @@
   </si>
   <si>
     <t>In-Progress</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -919,22 +927,22 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41065.0</c:v>
+                  <c:v>41065</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41078.0</c:v>
+                  <c:v>41078</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41092.0</c:v>
+                  <c:v>41092</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41106.0</c:v>
+                  <c:v>41106</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41120.0</c:v>
+                  <c:v>41120</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -946,19 +954,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -980,28 +988,28 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2031140440"/>
-        <c:axId val="2031137352"/>
+        <c:axId val="193137200"/>
+        <c:axId val="193137984"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2031140440"/>
+        <c:axId val="193137200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2031137352"/>
+        <c:crossAx val="193137984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2031137352"/>
+        <c:axId val="193137984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1012,7 +1020,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2031140440"/>
+        <c:crossAx val="193137200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1023,7 +1031,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1059,7 +1067,7 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41676.0</c:v>
+                  <c:v>41676</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1071,7 +1079,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1093,11 +1101,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2135677384"/>
-        <c:axId val="2135680456"/>
+        <c:axId val="70808384"/>
+        <c:axId val="70808776"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2135677384"/>
+        <c:axId val="70808384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1107,14 +1115,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2135680456"/>
+        <c:crossAx val="70808776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2135680456"/>
+        <c:axId val="70808776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1125,7 +1133,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2135677384"/>
+        <c:crossAx val="70808384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1136,7 +1144,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1963,15 +1971,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.453125" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" customWidth="1"/>
+    <col min="4" max="4" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -1985,7 +1993,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>172</v>
       </c>
@@ -1999,7 +2007,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>177</v>
       </c>
@@ -2013,7 +2021,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>182</v>
       </c>
@@ -2027,7 +2035,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>189</v>
       </c>
@@ -2041,7 +2049,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>190</v>
       </c>
@@ -2072,20 +2080,20 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.42578125" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.453125" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>175</v>
       </c>
@@ -2108,7 +2116,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30">
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -2131,7 +2139,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45">
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -2154,7 +2162,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="18">
         <v>3</v>
       </c>
@@ -2177,7 +2185,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="45">
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A5" s="18">
         <v>4</v>
       </c>
@@ -2200,7 +2208,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="18">
         <v>5</v>
       </c>
@@ -2223,7 +2231,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" s="18">
         <v>6</v>
       </c>
@@ -2246,7 +2254,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="60">
+    <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.2">
       <c r="A8" s="18">
         <v>7</v>
       </c>
@@ -2269,7 +2277,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30">
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A9" s="18">
         <v>8</v>
       </c>
@@ -2292,7 +2300,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="45">
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A10" s="18"/>
       <c r="B10" s="18"/>
       <c r="C10" s="18" t="s">
@@ -2307,7 +2315,7 @@
       <c r="F10" s="19"/>
       <c r="G10" s="18"/>
     </row>
-    <row r="11" spans="1:7" ht="30">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
       <c r="C11" s="18" t="s">
@@ -2322,7 +2330,7 @@
       <c r="F11" s="19"/>
       <c r="G11" s="18"/>
     </row>
-    <row r="12" spans="1:7" ht="30">
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="18"/>
       <c r="B12" s="18"/>
       <c r="C12" s="18" t="s">
@@ -2337,7 +2345,7 @@
       <c r="F12" s="19"/>
       <c r="G12" s="18"/>
     </row>
-    <row r="13" spans="1:7" ht="45">
+    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.2">
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
       <c r="C13" s="18" t="s">
@@ -2352,7 +2360,7 @@
       <c r="F13" s="19"/>
       <c r="G13" s="18"/>
     </row>
-    <row r="14" spans="1:7" ht="45">
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" s="18"/>
       <c r="B14" s="18"/>
       <c r="C14" s="18" t="s">
@@ -2367,7 +2375,7 @@
       <c r="F14" s="19"/>
       <c r="G14" s="18"/>
     </row>
-    <row r="15" spans="1:7" ht="45">
+    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.2">
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
       <c r="C15" s="18" t="s">
@@ -2382,7 +2390,7 @@
       <c r="F15" s="19"/>
       <c r="G15" s="18"/>
     </row>
-    <row r="16" spans="1:7" ht="30">
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" s="18"/>
       <c r="B16" s="18"/>
       <c r="C16" s="18" t="s">
@@ -2397,7 +2405,7 @@
       <c r="F16" s="19"/>
       <c r="G16" s="18"/>
     </row>
-    <row r="17" spans="3:6" ht="60">
+    <row r="17" spans="3:6" ht="60" x14ac:dyDescent="0.2">
       <c r="C17" s="18" t="s">
         <v>118</v>
       </c>
@@ -2409,7 +2417,7 @@
       </c>
       <c r="F17" s="19"/>
     </row>
-    <row r="18" spans="3:6" ht="90">
+    <row r="18" spans="3:6" ht="90" x14ac:dyDescent="0.2">
       <c r="C18" s="18" t="s">
         <v>119</v>
       </c>
@@ -2421,7 +2429,7 @@
       </c>
       <c r="F18" s="19"/>
     </row>
-    <row r="19" spans="3:6" ht="30">
+    <row r="19" spans="3:6" ht="30" x14ac:dyDescent="0.2">
       <c r="C19" s="18" t="s">
         <v>120</v>
       </c>
@@ -2433,7 +2441,7 @@
       </c>
       <c r="F19" s="19"/>
     </row>
-    <row r="20" spans="3:6" ht="30">
+    <row r="20" spans="3:6" ht="30" x14ac:dyDescent="0.2">
       <c r="C20" s="18" t="s">
         <v>121</v>
       </c>
@@ -2445,7 +2453,7 @@
       </c>
       <c r="F20" s="19"/>
     </row>
-    <row r="21" spans="3:6" ht="30">
+    <row r="21" spans="3:6" ht="30" x14ac:dyDescent="0.2">
       <c r="C21" s="18" t="s">
         <v>123</v>
       </c>
@@ -2457,7 +2465,7 @@
       </c>
       <c r="F21" s="19"/>
     </row>
-    <row r="22" spans="3:6" ht="30">
+    <row r="22" spans="3:6" ht="30" x14ac:dyDescent="0.2">
       <c r="C22" s="18" t="s">
         <v>124</v>
       </c>
@@ -2469,7 +2477,7 @@
       </c>
       <c r="F22" s="19"/>
     </row>
-    <row r="23" spans="3:6" ht="30">
+    <row r="23" spans="3:6" ht="30" x14ac:dyDescent="0.2">
       <c r="C23" s="18" t="s">
         <v>125</v>
       </c>
@@ -2481,7 +2489,7 @@
       </c>
       <c r="F23" s="19"/>
     </row>
-    <row r="24" spans="3:6" ht="30">
+    <row r="24" spans="3:6" ht="30" x14ac:dyDescent="0.2">
       <c r="C24" s="18" t="s">
         <v>126</v>
       </c>
@@ -2493,7 +2501,7 @@
       </c>
       <c r="F24" s="19"/>
     </row>
-    <row r="25" spans="3:6" ht="60">
+    <row r="25" spans="3:6" ht="60" x14ac:dyDescent="0.2">
       <c r="C25" s="18" t="s">
         <v>130</v>
       </c>
@@ -2505,7 +2513,7 @@
       </c>
       <c r="F25" s="19"/>
     </row>
-    <row r="26" spans="3:6" ht="45">
+    <row r="26" spans="3:6" ht="45" x14ac:dyDescent="0.2">
       <c r="C26" s="18" t="s">
         <v>131</v>
       </c>
@@ -2517,7 +2525,7 @@
       </c>
       <c r="F26" s="19"/>
     </row>
-    <row r="27" spans="3:6" ht="165">
+    <row r="27" spans="3:6" ht="180" x14ac:dyDescent="0.2">
       <c r="C27" s="18" t="s">
         <v>132</v>
       </c>
@@ -2529,7 +2537,7 @@
       </c>
       <c r="F27" s="19"/>
     </row>
-    <row r="28" spans="3:6" ht="30">
+    <row r="28" spans="3:6" ht="30" x14ac:dyDescent="0.2">
       <c r="C28" s="18" t="s">
         <v>133</v>
       </c>
@@ -2541,7 +2549,7 @@
       </c>
       <c r="F28" s="19"/>
     </row>
-    <row r="29" spans="3:6" ht="45">
+    <row r="29" spans="3:6" ht="45" x14ac:dyDescent="0.2">
       <c r="C29" s="18" t="s">
         <v>134</v>
       </c>
@@ -2553,7 +2561,7 @@
       </c>
       <c r="F29" s="19"/>
     </row>
-    <row r="30" spans="3:6" ht="30">
+    <row r="30" spans="3:6" ht="30" x14ac:dyDescent="0.2">
       <c r="C30" s="18" t="s">
         <v>135</v>
       </c>
@@ -2565,7 +2573,7 @@
       </c>
       <c r="F30" s="19"/>
     </row>
-    <row r="31" spans="3:6" ht="30">
+    <row r="31" spans="3:6" ht="30" x14ac:dyDescent="0.2">
       <c r="C31" s="18" t="s">
         <v>136</v>
       </c>
@@ -2577,7 +2585,7 @@
       </c>
       <c r="F31" s="19"/>
     </row>
-    <row r="32" spans="3:6" ht="45">
+    <row r="32" spans="3:6" ht="45" x14ac:dyDescent="0.2">
       <c r="C32" s="18" t="s">
         <v>137</v>
       </c>
@@ -2589,7 +2597,7 @@
       </c>
       <c r="F32" s="19"/>
     </row>
-    <row r="33" spans="3:6" ht="30">
+    <row r="33" spans="3:6" ht="30" x14ac:dyDescent="0.2">
       <c r="C33" s="18" t="s">
         <v>138</v>
       </c>
@@ -2622,47 +2630,47 @@
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="7"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>154</v>
       </c>
@@ -2685,7 +2693,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>155</v>
       </c>
@@ -2701,7 +2709,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>156</v>
       </c>
@@ -2726,7 +2734,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>157</v>
       </c>
@@ -2751,7 +2759,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>158</v>
       </c>
@@ -2776,7 +2784,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>159</v>
       </c>
@@ -2821,17 +2829,17 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11" style="2"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="16.7265625" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" customWidth="1"/>
+    <col min="5" max="5" width="7.1796875" customWidth="1"/>
+    <col min="6" max="6" width="6.81640625" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>154</v>
       </c>
@@ -2854,7 +2862,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>155</v>
       </c>
@@ -2883,23 +2891,23 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.28515625" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.26953125" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.26953125" customWidth="1"/>
+    <col min="8" max="8" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.453125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2928,7 +2936,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>128</v>
       </c>
@@ -2945,7 +2953,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
         <v>129</v>
       </c>
@@ -2962,7 +2970,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>122</v>
       </c>
@@ -2979,7 +2987,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
         <v>107</v>
       </c>
@@ -2995,8 +3003,17 @@
       <c r="F5">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="G5">
+        <v>13</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
         <v>108</v>
       </c>
@@ -3012,8 +3029,17 @@
       <c r="F6">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="G6">
+        <v>9</v>
+      </c>
+      <c r="H6">
+        <v>15</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
         <v>109</v>
       </c>
@@ -3030,7 +3056,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
         <v>113</v>
       </c>
@@ -3047,7 +3073,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
         <v>127</v>
       </c>
@@ -3064,21 +3090,21 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="5"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="2:2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
         <v>26</v>
       </c>
@@ -3104,9 +3130,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3155,9 +3181,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3205,9 +3231,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3253,13 +3279,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>106</v>
       </c>
@@ -3270,7 +3296,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -3281,7 +3307,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -3292,7 +3318,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -3303,7 +3329,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -3314,7 +3340,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>111</v>
       </c>
@@ -3325,7 +3351,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -3336,7 +3362,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>113</v>
       </c>
@@ -3347,7 +3373,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -3358,7 +3384,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>115</v>
       </c>
@@ -3369,7 +3395,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>116</v>
       </c>
@@ -3380,7 +3406,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>117</v>
       </c>
@@ -3391,7 +3417,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>118</v>
       </c>
@@ -3402,7 +3428,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="45">
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>119</v>
       </c>
@@ -3413,7 +3439,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>120</v>
       </c>
@@ -3424,7 +3450,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>121</v>
       </c>
@@ -3435,7 +3461,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>122</v>
       </c>
@@ -3446,7 +3472,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>123</v>
       </c>
@@ -3457,7 +3483,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>124</v>
       </c>
@@ -3468,7 +3494,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>125</v>
       </c>
@@ -3479,7 +3505,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15">
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>126</v>
       </c>
@@ -3490,7 +3516,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>127</v>
       </c>
@@ -3501,7 +3527,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>128</v>
       </c>
@@ -3512,7 +3538,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>129</v>
       </c>
@@ -3523,7 +3549,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>130</v>
       </c>
@@ -3534,7 +3560,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>131</v>
       </c>
@@ -3545,7 +3571,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="90">
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>132</v>
       </c>
@@ -3556,7 +3582,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>133</v>
       </c>
@@ -3567,7 +3593,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>134</v>
       </c>
@@ -3578,7 +3604,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>135</v>
       </c>
@@ -3589,7 +3615,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>136</v>
       </c>
@@ -3600,7 +3626,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>137</v>
       </c>
@@ -3611,7 +3637,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>138</v>
       </c>
@@ -3622,7 +3648,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>139</v>
       </c>
@@ -3633,7 +3659,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>140</v>
       </c>
@@ -3644,7 +3670,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>141</v>
       </c>
@@ -3655,7 +3681,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15">
+    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>142</v>
       </c>
@@ -3666,7 +3692,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>143</v>
       </c>
@@ -3677,7 +3703,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>144</v>
       </c>
@@ -3688,7 +3714,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>145</v>
       </c>
@@ -3699,7 +3725,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>146</v>
       </c>
@@ -3710,7 +3736,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>147</v>
       </c>
@@ -3721,7 +3747,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>148</v>
       </c>

</xml_diff>

<commit_message>
Update latest sprint status
</commit_message>
<xml_diff>
--- a/TeamEstherKarelKeithTroyReport.xlsx
+++ b/TeamEstherKarelKeithTroyReport.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28705"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esthe\OneDrive\Documents\GitHub\stevens_cs555\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-15" windowWidth="28800" windowHeight="16425" tabRatio="627" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="16420" tabRatio="627" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -24,9 +19,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backlog!$A$1:$F$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sprint1!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sprint1!$A$1:$I$16</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -639,9 +639,6 @@
     <t>Est Size (lines of code)</t>
   </si>
   <si>
-    <t>See Project Board</t>
-  </si>
-  <si>
     <t>T16.01</t>
   </si>
   <si>
@@ -682,12 +679,15 @@
   </si>
   <si>
     <t>Completed</t>
+  </si>
+  <si>
+    <t>See Git Project Board</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -750,7 +750,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="69">
+  <cellStyleXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -820,6 +820,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -876,7 +878,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="69">
+  <cellStyles count="71">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -910,6 +912,8 @@
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -961,7 +965,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -987,22 +991,22 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41065</c:v>
+                  <c:v>41065.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41078</c:v>
+                  <c:v>41078.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41092</c:v>
+                  <c:v>41092.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41106</c:v>
+                  <c:v>41106.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41120</c:v>
+                  <c:v>41120.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1014,25 +1018,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8005-41C3-A2A6-994BE20B6C54}"/>
             </c:ext>
@@ -1048,28 +1052,28 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2135732552"/>
-        <c:axId val="2135735624"/>
+        <c:axId val="-2131947880"/>
+        <c:axId val="-2131944808"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2135732552"/>
+        <c:axId val="-2131947880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2135735624"/>
+        <c:crossAx val="-2131944808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2135735624"/>
+        <c:axId val="-2131944808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1080,7 +1084,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2135732552"/>
+        <c:crossAx val="-2131947880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1091,14 +1095,14 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1127,7 +1131,7 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41676</c:v>
+                  <c:v>41676.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1139,13 +1143,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5A9F-42BD-9352-89747C7C9AC0}"/>
             </c:ext>
@@ -1161,11 +1165,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2137451944"/>
-        <c:axId val="2137455016"/>
+        <c:axId val="-2138774120"/>
+        <c:axId val="-2138777208"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2137451944"/>
+        <c:axId val="-2138774120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1175,14 +1179,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2137455016"/>
+        <c:crossAx val="-2138777208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2137455016"/>
+        <c:axId val="-2138777208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1193,7 +1197,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2137451944"/>
+        <c:crossAx val="-2138774120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1204,7 +1208,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1230,7 +1234,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1268,7 +1272,7 @@
         <xdr:cNvPr id="3" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1343,7 +1347,7 @@
         <xdr:cNvPr id="4" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1408,7 +1412,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1477,7 +1481,7 @@
         <xdr:cNvPr id="6" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1547,7 +1551,7 @@
         <xdr:cNvPr id="7" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1616,7 +1620,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1686,7 +1690,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2031,15 +2035,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.375" customWidth="1"/>
-    <col min="3" max="3" width="10.875" customWidth="1"/>
-    <col min="4" max="4" width="20.375" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -2053,7 +2057,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>172</v>
       </c>
@@ -2067,7 +2071,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>177</v>
       </c>
@@ -2081,7 +2085,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>182</v>
       </c>
@@ -2095,7 +2099,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>189</v>
       </c>
@@ -2109,7 +2113,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="C9" t="s">
         <v>190</v>
       </c>
@@ -2139,21 +2143,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.375" customWidth="1"/>
-    <col min="7" max="7" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" s="17" t="s">
         <v>175</v>
       </c>
@@ -2176,7 +2180,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="30">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -2196,10 +2200,10 @@
         <v>172</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="63" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="45">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -2222,7 +2226,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="30">
       <c r="A4" s="18">
         <v>3</v>
       </c>
@@ -2242,10 +2246,10 @@
         <v>177</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="45">
       <c r="A5" s="18">
         <v>4</v>
       </c>
@@ -2268,7 +2272,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="30">
       <c r="A6" s="18">
         <v>5</v>
       </c>
@@ -2291,7 +2295,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="30">
       <c r="A7" s="18">
         <v>6</v>
       </c>
@@ -2314,7 +2318,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="94.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="60">
       <c r="A8" s="18">
         <v>7</v>
       </c>
@@ -2334,10 +2338,10 @@
         <v>177</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30">
       <c r="A9" s="18">
         <v>8</v>
       </c>
@@ -2360,7 +2364,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="220.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="165">
       <c r="A10" s="25">
         <v>9</v>
       </c>
@@ -2377,7 +2381,7 @@
       <c r="F10" s="19"/>
       <c r="G10" s="25"/>
     </row>
-    <row r="11" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="30">
       <c r="A11" s="25">
         <v>10</v>
       </c>
@@ -2394,7 +2398,7 @@
       <c r="F11" s="19"/>
       <c r="G11" s="25"/>
     </row>
-    <row r="12" spans="1:7" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="60">
       <c r="A12" s="25">
         <v>11</v>
       </c>
@@ -2411,7 +2415,7 @@
       <c r="F12" s="19"/>
       <c r="G12" s="25"/>
     </row>
-    <row r="13" spans="1:7" ht="63" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="45">
       <c r="A13" s="18">
         <v>12</v>
       </c>
@@ -2428,7 +2432,7 @@
       <c r="F13" s="19"/>
       <c r="G13" s="18"/>
     </row>
-    <row r="14" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="45">
       <c r="A14" s="18">
         <v>13</v>
       </c>
@@ -2445,7 +2449,7 @@
       <c r="F14" s="19"/>
       <c r="G14" s="18"/>
     </row>
-    <row r="15" spans="1:7" ht="63" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="45">
       <c r="A15" s="18">
         <v>14</v>
       </c>
@@ -2462,7 +2466,7 @@
       <c r="F15" s="19"/>
       <c r="G15" s="18"/>
     </row>
-    <row r="16" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="30">
       <c r="A16" s="18">
         <v>15</v>
       </c>
@@ -2479,7 +2483,7 @@
       <c r="F16" s="19"/>
       <c r="G16" s="18"/>
     </row>
-    <row r="17" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="30">
       <c r="A17" s="18">
         <v>16</v>
       </c>
@@ -2496,7 +2500,7 @@
       <c r="F17" s="19"/>
       <c r="G17" s="18"/>
     </row>
-    <row r="18" spans="1:7" ht="63" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="45">
       <c r="A18" s="18">
         <v>17</v>
       </c>
@@ -2513,7 +2517,7 @@
       <c r="F18" s="19"/>
       <c r="G18" s="18"/>
     </row>
-    <row r="19" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="30">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2528,7 +2532,7 @@
       </c>
       <c r="F19" s="19"/>
     </row>
-    <row r="20" spans="1:7" ht="110.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="90">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2543,7 +2547,7 @@
       </c>
       <c r="F20" s="19"/>
     </row>
-    <row r="21" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="30">
       <c r="A21" s="18">
         <v>20</v>
       </c>
@@ -2560,7 +2564,7 @@
       <c r="F21" s="19"/>
       <c r="G21" s="18"/>
     </row>
-    <row r="22" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="30">
       <c r="A22" s="25">
         <v>21</v>
       </c>
@@ -2577,7 +2581,7 @@
       <c r="F22" s="19"/>
       <c r="G22" s="25"/>
     </row>
-    <row r="23" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="30">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2592,7 +2596,7 @@
       </c>
       <c r="F23" s="19"/>
     </row>
-    <row r="24" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="30">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2607,7 +2611,7 @@
       </c>
       <c r="F24" s="19"/>
     </row>
-    <row r="25" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="30">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2622,7 +2626,7 @@
       </c>
       <c r="F25" s="19"/>
     </row>
-    <row r="26" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="45">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2637,7 +2641,7 @@
       </c>
       <c r="F26" s="19"/>
     </row>
-    <row r="27" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="30">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2652,7 +2656,7 @@
       </c>
       <c r="F27" s="19"/>
     </row>
-    <row r="28" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="45">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2667,7 +2671,7 @@
       </c>
       <c r="F28" s="19"/>
     </row>
-    <row r="29" spans="1:7" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="60">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2682,7 +2686,7 @@
       </c>
       <c r="F29" s="19"/>
     </row>
-    <row r="30" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="30">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2697,7 +2701,7 @@
       </c>
       <c r="F30" s="19"/>
     </row>
-    <row r="31" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="45">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2712,7 +2716,7 @@
       </c>
       <c r="F31" s="19"/>
     </row>
-    <row r="32" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="30">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2727,7 +2731,7 @@
       </c>
       <c r="F32" s="19"/>
     </row>
-    <row r="33" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="30">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2766,47 +2770,47 @@
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11" style="7"/>
-    <col min="2" max="2" width="9.375" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.25" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" s="7" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="7" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="7" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" s="7" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="4" customFormat="1">
       <c r="A14" s="4" t="s">
         <v>154</v>
       </c>
@@ -2829,7 +2833,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>155</v>
       </c>
@@ -2845,7 +2849,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>156</v>
       </c>
@@ -2870,7 +2874,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" s="7" t="s">
         <v>157</v>
       </c>
@@ -2895,7 +2899,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" s="7" t="s">
         <v>158</v>
       </c>
@@ -2920,7 +2924,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" s="7" t="s">
         <v>159</v>
       </c>
@@ -2965,17 +2969,17 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="11" style="2"/>
-    <col min="3" max="3" width="16.75" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="7.125" customWidth="1"/>
-    <col min="6" max="6" width="6.875" customWidth="1"/>
-    <col min="7" max="7" width="12.375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>154</v>
       </c>
@@ -2998,7 +3002,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>155</v>
       </c>
@@ -3026,24 +3030,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.25" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.28515625" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.5" style="26" customWidth="1"/>
-    <col min="3" max="3" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.625" customWidth="1"/>
-    <col min="5" max="5" width="24.625" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" style="26" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.25" customWidth="1"/>
-    <col min="8" max="8" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3072,7 +3076,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="18" t="s">
         <v>128</v>
       </c>
@@ -3082,8 +3086,8 @@
       <c r="C2" t="s">
         <v>172</v>
       </c>
-      <c r="D2" t="s">
-        <v>194</v>
+      <c r="D2" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -3091,8 +3095,17 @@
       <c r="F2">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>30</v>
+      </c>
+      <c r="I2" s="6">
+        <v>41682</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="18" t="s">
         <v>129</v>
       </c>
@@ -3102,8 +3115,8 @@
       <c r="C3" t="s">
         <v>182</v>
       </c>
-      <c r="D3" t="s">
-        <v>194</v>
+      <c r="D3" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="E3">
         <v>12</v>
@@ -3112,7 +3125,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="18" t="s">
         <v>122</v>
       </c>
@@ -3122,8 +3135,8 @@
       <c r="C4" t="s">
         <v>177</v>
       </c>
-      <c r="D4" t="s">
-        <v>194</v>
+      <c r="D4" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="E4">
         <v>5</v>
@@ -3141,75 +3154,75 @@
         <v>41678</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="26">
       <c r="A5" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C5" t="s">
         <v>177</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="I5" s="27">
         <v>41678</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="26">
       <c r="A6" s="22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C6" t="s">
         <v>177</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="I6" s="27">
         <v>41678</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="26">
       <c r="A7" s="22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C7" t="s">
         <v>177</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="I7" s="27">
         <v>41678</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="26">
       <c r="A8" s="22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C8" t="s">
         <v>177</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="I8" s="27">
         <v>41678</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" s="18" t="s">
         <v>107</v>
       </c>
@@ -3219,8 +3232,8 @@
       <c r="C9" t="s">
         <v>189</v>
       </c>
-      <c r="D9" t="s">
-        <v>194</v>
+      <c r="D9" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="E9">
         <v>5</v>
@@ -3238,7 +3251,7 @@
         <v>41681</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" s="18" t="s">
         <v>108</v>
       </c>
@@ -3248,8 +3261,8 @@
       <c r="C10" t="s">
         <v>189</v>
       </c>
-      <c r="D10" t="s">
-        <v>194</v>
+      <c r="D10" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="E10">
         <v>5</v>
@@ -3267,7 +3280,7 @@
         <v>41681</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" s="18" t="s">
         <v>109</v>
       </c>
@@ -3277,8 +3290,8 @@
       <c r="C11" t="s">
         <v>172</v>
       </c>
-      <c r="D11" t="s">
-        <v>194</v>
+      <c r="D11" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="E11">
         <v>10</v>
@@ -3287,7 +3300,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12" s="18" t="s">
         <v>113</v>
       </c>
@@ -3297,8 +3310,8 @@
       <c r="C12" t="s">
         <v>177</v>
       </c>
-      <c r="D12" t="s">
-        <v>194</v>
+      <c r="D12" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="E12">
         <v>20</v>
@@ -3316,58 +3329,58 @@
         <v>41680</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" s="21" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C13" s="25" t="s">
         <v>177</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="I13" s="27">
         <v>41680</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="25" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" s="25" customFormat="1" ht="26">
       <c r="A14" s="21" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C14" s="25" t="s">
         <v>177</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="I14" s="27">
         <v>41680</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="26">
       <c r="A15" s="21" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C15" s="25" t="s">
         <v>177</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="I15" s="27">
         <v>41680</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="A16" s="18" t="s">
         <v>127</v>
       </c>
@@ -3377,8 +3390,8 @@
       <c r="C16" t="s">
         <v>182</v>
       </c>
-      <c r="D16" t="s">
-        <v>194</v>
+      <c r="D16" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="E16">
         <v>10</v>
@@ -3387,30 +3400,35 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:9">
       <c r="B21" s="28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:9">
       <c r="B22" s="28"/>
       <c r="I22" s="7"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:9">
       <c r="B23" s="28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:9">
       <c r="B27" s="28" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I1"/>
+  <autoFilter ref="A1:I16"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3422,9 +3440,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3473,9 +3491,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3523,9 +3541,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3571,13 +3589,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>106</v>
       </c>
@@ -3588,7 +3606,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="30">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -3599,7 +3617,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="15">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -3610,7 +3628,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="15">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -3621,7 +3639,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="30">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -3632,7 +3650,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="15">
       <c r="A6" t="s">
         <v>111</v>
       </c>
@@ -3643,7 +3661,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="15">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -3654,7 +3672,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="45">
       <c r="A8" t="s">
         <v>113</v>
       </c>
@@ -3665,7 +3683,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="30">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -3676,7 +3694,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="30">
       <c r="A10" t="s">
         <v>115</v>
       </c>
@@ -3687,7 +3705,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="30">
       <c r="A11" t="s">
         <v>116</v>
       </c>
@@ -3698,7 +3716,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="15">
       <c r="A12" t="s">
         <v>117</v>
       </c>
@@ -3709,7 +3727,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="30">
       <c r="A13" t="s">
         <v>118</v>
       </c>
@@ -3720,7 +3738,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="45">
       <c r="A14" t="s">
         <v>119</v>
       </c>
@@ -3731,7 +3749,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="15">
       <c r="A15" t="s">
         <v>120</v>
       </c>
@@ -3742,7 +3760,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="15">
       <c r="A16" t="s">
         <v>121</v>
       </c>
@@ -3753,7 +3771,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="15">
       <c r="A17" t="s">
         <v>122</v>
       </c>
@@ -3764,7 +3782,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="15">
       <c r="A18" t="s">
         <v>123</v>
       </c>
@@ -3775,7 +3793,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15">
       <c r="A19" t="s">
         <v>124</v>
       </c>
@@ -3786,7 +3804,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15">
       <c r="A20" t="s">
         <v>125</v>
       </c>
@@ -3797,7 +3815,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="15">
       <c r="A21" t="s">
         <v>126</v>
       </c>
@@ -3808,7 +3826,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="30">
       <c r="A22" t="s">
         <v>127</v>
       </c>
@@ -3819,7 +3837,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="30">
       <c r="A23" t="s">
         <v>128</v>
       </c>
@@ -3830,7 +3848,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="30">
       <c r="A24" t="s">
         <v>129</v>
       </c>
@@ -3841,7 +3859,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="30">
       <c r="A25" t="s">
         <v>130</v>
       </c>
@@ -3852,7 +3870,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="30">
       <c r="A26" t="s">
         <v>131</v>
       </c>
@@ -3863,7 +3881,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="126" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="90">
       <c r="A27" t="s">
         <v>132</v>
       </c>
@@ -3874,7 +3892,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="15">
       <c r="A28" t="s">
         <v>133</v>
       </c>
@@ -3885,7 +3903,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="30">
       <c r="A29" t="s">
         <v>134</v>
       </c>
@@ -3896,7 +3914,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="15">
       <c r="A30" t="s">
         <v>135</v>
       </c>
@@ -3907,7 +3925,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="15">
       <c r="A31" t="s">
         <v>136</v>
       </c>
@@ -3918,7 +3936,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="30">
       <c r="A32" t="s">
         <v>137</v>
       </c>
@@ -3929,7 +3947,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="15">
       <c r="A33" t="s">
         <v>138</v>
       </c>
@@ -3940,7 +3958,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="30">
       <c r="A34" t="s">
         <v>139</v>
       </c>
@@ -3951,7 +3969,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="30">
       <c r="A35" t="s">
         <v>140</v>
       </c>
@@ -3962,7 +3980,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="30">
       <c r="A36" t="s">
         <v>141</v>
       </c>
@@ -3973,7 +3991,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="15">
       <c r="A37" t="s">
         <v>142</v>
       </c>
@@ -3984,7 +4002,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="30">
       <c r="A38" t="s">
         <v>143</v>
       </c>
@@ -3995,7 +4013,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="30">
       <c r="A39" t="s">
         <v>144</v>
       </c>
@@ -4006,7 +4024,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="30">
       <c r="A40" t="s">
         <v>145</v>
       </c>
@@ -4017,7 +4035,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="30">
       <c r="A41" t="s">
         <v>146</v>
       </c>
@@ -4028,7 +4046,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="15">
       <c r="A42" t="s">
         <v>147</v>
       </c>
@@ -4039,7 +4057,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="30">
       <c r="A43" t="s">
         <v>148</v>
       </c>

</xml_diff>

<commit_message>
Updated US23 metrics for Sprint 1
</commit_message>
<xml_diff>
--- a/TeamEstherKarelKeithTroyReport.xlsx
+++ b/TeamEstherKarelKeithTroyReport.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28705"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="16420" tabRatio="627" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="-15" windowWidth="28800" windowHeight="16425" tabRatio="627" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backlog!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sprint1!$A$1:$I$16</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -991,22 +991,22 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41065.0</c:v>
+                  <c:v>41065</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41078.0</c:v>
+                  <c:v>41078</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41092.0</c:v>
+                  <c:v>41092</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41106.0</c:v>
+                  <c:v>41106</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41120.0</c:v>
+                  <c:v>41120</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1018,19 +1018,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1052,28 +1052,28 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2131947880"/>
-        <c:axId val="-2131944808"/>
+        <c:axId val="61242752"/>
+        <c:axId val="61269120"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-2131947880"/>
+        <c:axId val="61242752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131944808"/>
+        <c:crossAx val="61269120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2131944808"/>
+        <c:axId val="61269120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1084,7 +1084,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131947880"/>
+        <c:crossAx val="61242752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1095,7 +1095,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1131,7 +1131,7 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41676.0</c:v>
+                  <c:v>41676</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1143,7 +1143,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1165,11 +1165,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2138774120"/>
-        <c:axId val="-2138777208"/>
+        <c:axId val="129753856"/>
+        <c:axId val="129755392"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-2138774120"/>
+        <c:axId val="129753856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1179,14 +1179,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2138777208"/>
+        <c:crossAx val="129755392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2138777208"/>
+        <c:axId val="129755392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1197,7 +1197,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2138774120"/>
+        <c:crossAx val="129753856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1208,7 +1208,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1234,7 +1234,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1272,7 +1272,7 @@
         <xdr:cNvPr id="3" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1347,7 +1347,7 @@
         <xdr:cNvPr id="4" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1412,7 +1412,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1481,7 +1481,7 @@
         <xdr:cNvPr id="6" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1551,7 +1551,7 @@
         <xdr:cNvPr id="7" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1620,7 +1620,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1690,7 +1690,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2035,15 +2035,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.375" customWidth="1"/>
+    <col min="3" max="3" width="10.875" customWidth="1"/>
+    <col min="4" max="4" width="20.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>172</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>177</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>182</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>189</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>190</v>
       </c>
@@ -2143,21 +2143,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.42578125" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.375" customWidth="1"/>
+    <col min="7" max="7" width="9.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>175</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30">
+    <row r="2" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -2203,7 +2203,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45">
+    <row r="3" spans="1:7" ht="63" x14ac:dyDescent="0.2">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30">
+    <row r="4" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A4" s="18">
         <v>3</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="45">
+    <row r="5" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A5" s="18">
         <v>4</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30">
+    <row r="6" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A6" s="18">
         <v>5</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30">
+    <row r="7" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A7" s="18">
         <v>6</v>
       </c>
@@ -2318,7 +2318,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="60">
+    <row r="8" spans="1:7" ht="78.75" x14ac:dyDescent="0.2">
       <c r="A8" s="18">
         <v>7</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30">
+    <row r="9" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A9" s="18">
         <v>8</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="165">
+    <row r="10" spans="1:7" ht="204.75" x14ac:dyDescent="0.2">
       <c r="A10" s="25">
         <v>9</v>
       </c>
@@ -2381,7 +2381,7 @@
       <c r="F10" s="19"/>
       <c r="G10" s="25"/>
     </row>
-    <row r="11" spans="1:7" ht="30">
+    <row r="11" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A11" s="25">
         <v>10</v>
       </c>
@@ -2398,7 +2398,7 @@
       <c r="F11" s="19"/>
       <c r="G11" s="25"/>
     </row>
-    <row r="12" spans="1:7" ht="60">
+    <row r="12" spans="1:7" ht="78.75" x14ac:dyDescent="0.2">
       <c r="A12" s="25">
         <v>11</v>
       </c>
@@ -2415,7 +2415,7 @@
       <c r="F12" s="19"/>
       <c r="G12" s="25"/>
     </row>
-    <row r="13" spans="1:7" ht="45">
+    <row r="13" spans="1:7" ht="63" x14ac:dyDescent="0.2">
       <c r="A13" s="18">
         <v>12</v>
       </c>
@@ -2432,7 +2432,7 @@
       <c r="F13" s="19"/>
       <c r="G13" s="18"/>
     </row>
-    <row r="14" spans="1:7" ht="45">
+    <row r="14" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A14" s="18">
         <v>13</v>
       </c>
@@ -2449,7 +2449,7 @@
       <c r="F14" s="19"/>
       <c r="G14" s="18"/>
     </row>
-    <row r="15" spans="1:7" ht="45">
+    <row r="15" spans="1:7" ht="63" x14ac:dyDescent="0.2">
       <c r="A15" s="18">
         <v>14</v>
       </c>
@@ -2466,7 +2466,7 @@
       <c r="F15" s="19"/>
       <c r="G15" s="18"/>
     </row>
-    <row r="16" spans="1:7" ht="30">
+    <row r="16" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A16" s="18">
         <v>15</v>
       </c>
@@ -2483,7 +2483,7 @@
       <c r="F16" s="19"/>
       <c r="G16" s="18"/>
     </row>
-    <row r="17" spans="1:7" ht="30">
+    <row r="17" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A17" s="18">
         <v>16</v>
       </c>
@@ -2500,7 +2500,7 @@
       <c r="F17" s="19"/>
       <c r="G17" s="18"/>
     </row>
-    <row r="18" spans="1:7" ht="45">
+    <row r="18" spans="1:7" ht="63" x14ac:dyDescent="0.2">
       <c r="A18" s="18">
         <v>17</v>
       </c>
@@ -2517,7 +2517,7 @@
       <c r="F18" s="19"/>
       <c r="G18" s="18"/>
     </row>
-    <row r="19" spans="1:7" ht="30">
+    <row r="19" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2532,7 +2532,7 @@
       </c>
       <c r="F19" s="19"/>
     </row>
-    <row r="20" spans="1:7" ht="90">
+    <row r="20" spans="1:7" ht="110.25" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2547,7 +2547,7 @@
       </c>
       <c r="F20" s="19"/>
     </row>
-    <row r="21" spans="1:7" ht="30">
+    <row r="21" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A21" s="18">
         <v>20</v>
       </c>
@@ -2564,7 +2564,7 @@
       <c r="F21" s="19"/>
       <c r="G21" s="18"/>
     </row>
-    <row r="22" spans="1:7" ht="30">
+    <row r="22" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A22" s="25">
         <v>21</v>
       </c>
@@ -2581,7 +2581,7 @@
       <c r="F22" s="19"/>
       <c r="G22" s="25"/>
     </row>
-    <row r="23" spans="1:7" ht="30">
+    <row r="23" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2596,7 +2596,7 @@
       </c>
       <c r="F23" s="19"/>
     </row>
-    <row r="24" spans="1:7" ht="30">
+    <row r="24" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2611,7 +2611,7 @@
       </c>
       <c r="F24" s="19"/>
     </row>
-    <row r="25" spans="1:7" ht="30">
+    <row r="25" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2626,7 +2626,7 @@
       </c>
       <c r="F25" s="19"/>
     </row>
-    <row r="26" spans="1:7" ht="45">
+    <row r="26" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2641,7 +2641,7 @@
       </c>
       <c r="F26" s="19"/>
     </row>
-    <row r="27" spans="1:7" ht="30">
+    <row r="27" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2656,7 +2656,7 @@
       </c>
       <c r="F27" s="19"/>
     </row>
-    <row r="28" spans="1:7" ht="45">
+    <row r="28" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2671,7 +2671,7 @@
       </c>
       <c r="F28" s="19"/>
     </row>
-    <row r="29" spans="1:7" ht="60">
+    <row r="29" spans="1:7" ht="78.75" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2686,7 +2686,7 @@
       </c>
       <c r="F29" s="19"/>
     </row>
-    <row r="30" spans="1:7" ht="30">
+    <row r="30" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2701,7 +2701,7 @@
       </c>
       <c r="F30" s="19"/>
     </row>
-    <row r="31" spans="1:7" ht="45">
+    <row r="31" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2716,7 +2716,7 @@
       </c>
       <c r="F31" s="19"/>
     </row>
-    <row r="32" spans="1:7" ht="30">
+    <row r="32" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2731,7 +2731,7 @@
       </c>
       <c r="F32" s="19"/>
     </row>
-    <row r="33" spans="1:6" ht="30">
+    <row r="33" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2770,47 +2770,47 @@
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="7"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="9.375" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.25" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="12.375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>154</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>155</v>
       </c>
@@ -2849,7 +2849,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>156</v>
       </c>
@@ -2874,7 +2874,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>157</v>
       </c>
@@ -2899,7 +2899,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>158</v>
       </c>
@@ -2924,7 +2924,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>159</v>
       </c>
@@ -2969,17 +2969,17 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11" style="2"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="16.75" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="5" max="5" width="7.125" customWidth="1"/>
+    <col min="6" max="6" width="6.875" customWidth="1"/>
+    <col min="7" max="7" width="12.375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>154</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>155</v>
       </c>
@@ -3030,24 +3030,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.28515625" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.25" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" style="26" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.375" style="26" customWidth="1"/>
+    <col min="3" max="3" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.625" customWidth="1"/>
+    <col min="5" max="5" width="24.625" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="13.25" customWidth="1"/>
+    <col min="8" max="8" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3076,7 +3074,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>128</v>
       </c>
@@ -3105,7 +3103,7 @@
         <v>41682</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
         <v>129</v>
       </c>
@@ -3124,8 +3122,14 @@
       <c r="F3">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="G3">
+        <v>25</v>
+      </c>
+      <c r="H3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>122</v>
       </c>
@@ -3154,7 +3158,7 @@
         <v>41678</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="26">
+    <row r="5" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
         <v>194</v>
       </c>
@@ -3171,7 +3175,7 @@
         <v>41678</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="26">
+    <row r="6" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
         <v>195</v>
       </c>
@@ -3188,7 +3192,7 @@
         <v>41678</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="26">
+    <row r="7" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
         <v>196</v>
       </c>
@@ -3205,7 +3209,7 @@
         <v>41678</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="26">
+    <row r="8" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
         <v>196</v>
       </c>
@@ -3222,7 +3226,7 @@
         <v>41678</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
         <v>107</v>
       </c>
@@ -3251,7 +3255,7 @@
         <v>41681</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
         <v>108</v>
       </c>
@@ -3280,7 +3284,7 @@
         <v>41681</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
         <v>109</v>
       </c>
@@ -3300,7 +3304,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
         <v>113</v>
       </c>
@@ -3329,7 +3333,7 @@
         <v>41680</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="21" t="s">
         <v>201</v>
       </c>
@@ -3346,7 +3350,7 @@
         <v>41680</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="25" customFormat="1" ht="26">
+    <row r="14" spans="1:9" s="25" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="s">
         <v>202</v>
       </c>
@@ -3363,7 +3367,7 @@
         <v>41680</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="26">
+    <row r="15" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
         <v>203</v>
       </c>
@@ -3380,7 +3384,7 @@
         <v>41680</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
         <v>127</v>
       </c>
@@ -3400,21 +3404,21 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="2:9">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B21" s="28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="2:9">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" s="28"/>
       <c r="I22" s="7"/>
     </row>
-    <row r="23" spans="2:9">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B23" s="28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="2:9">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B27" s="28" t="s">
         <v>26</v>
       </c>
@@ -3440,9 +3444,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3491,9 +3495,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3541,9 +3545,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3589,13 +3593,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>106</v>
       </c>
@@ -3606,7 +3610,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30">
+    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -3617,7 +3621,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15">
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -3628,7 +3632,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -3639,7 +3643,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30">
+    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -3650,7 +3654,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15">
+    <row r="6" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>111</v>
       </c>
@@ -3661,7 +3665,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15">
+    <row r="7" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -3672,7 +3676,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45">
+    <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>113</v>
       </c>
@@ -3683,7 +3687,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30">
+    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -3694,7 +3698,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30">
+    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>115</v>
       </c>
@@ -3705,7 +3709,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30">
+    <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>116</v>
       </c>
@@ -3716,7 +3720,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15">
+    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>117</v>
       </c>
@@ -3727,7 +3731,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30">
+    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>118</v>
       </c>
@@ -3738,7 +3742,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="45">
+    <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>119</v>
       </c>
@@ -3749,7 +3753,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15">
+    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>120</v>
       </c>
@@ -3760,7 +3764,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15">
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>121</v>
       </c>
@@ -3771,7 +3775,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15">
+    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>122</v>
       </c>
@@ -3782,7 +3786,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15">
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>123</v>
       </c>
@@ -3793,7 +3797,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15">
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>124</v>
       </c>
@@ -3804,7 +3808,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15">
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>125</v>
       </c>
@@ -3815,7 +3819,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15">
+    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>126</v>
       </c>
@@ -3826,7 +3830,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30">
+    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>127</v>
       </c>
@@ -3837,7 +3841,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30">
+    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>128</v>
       </c>
@@ -3848,7 +3852,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30">
+    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>129</v>
       </c>
@@ -3859,7 +3863,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30">
+    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>130</v>
       </c>
@@ -3870,7 +3874,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30">
+    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>131</v>
       </c>
@@ -3881,7 +3885,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="90">
+    <row r="27" spans="1:3" ht="126" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>132</v>
       </c>
@@ -3892,7 +3896,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15">
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>133</v>
       </c>
@@ -3903,7 +3907,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30">
+    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>134</v>
       </c>
@@ -3914,7 +3918,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15">
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>135</v>
       </c>
@@ -3925,7 +3929,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15">
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>136</v>
       </c>
@@ -3936,7 +3940,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30">
+    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>137</v>
       </c>
@@ -3947,7 +3951,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15">
+    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>138</v>
       </c>
@@ -3958,7 +3962,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30">
+    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>139</v>
       </c>
@@ -3969,7 +3973,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30">
+    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>140</v>
       </c>
@@ -3980,7 +3984,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30">
+    <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>141</v>
       </c>
@@ -3991,7 +3995,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15">
+    <row r="37" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>142</v>
       </c>
@@ -4002,7 +4006,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30">
+    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>143</v>
       </c>
@@ -4013,7 +4017,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30">
+    <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>144</v>
       </c>
@@ -4024,7 +4028,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30">
+    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>145</v>
       </c>
@@ -4035,7 +4039,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30">
+    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>146</v>
       </c>
@@ -4046,7 +4050,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15">
+    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>147</v>
       </c>
@@ -4057,7 +4061,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30">
+    <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>148</v>
       </c>

</xml_diff>

<commit_message>
Updated burndown, Sprint 1 and Sprint 2 stories
</commit_message>
<xml_diff>
--- a/TeamEstherKarelKeithTroyReport.xlsx
+++ b/TeamEstherKarelKeithTroyReport.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esthe\OneDrive\Documents\GitHub\stevens_cs555\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klros\Google Drive\Keith\Stevens Institute of Technology\SSW-555-WS\gedcom\stevens_cs555\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-15" windowWidth="28800" windowHeight="16425" tabRatio="627" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="16430" tabRatio="627" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backlog!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sprint1!$A$1:$I$16</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="220">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -717,12 +717,15 @@
   </si>
   <si>
     <t>fix individual.py should make sure there is a spouse before adding spouse, instead of making sure there are children before adding spouse</t>
+  </si>
+  <si>
+    <t>not started</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -996,7 +999,7 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="68"/>
+    <cellStyle name="Normal 2" xfId="68" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1183,6 +1186,15 @@
                 <c:pt idx="1">
                   <c:v>41696</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>41717</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41731</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41745</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1197,6 +1209,15 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2083,20 +2104,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.375" customWidth="1"/>
-    <col min="3" max="3" width="10.875" customWidth="1"/>
-    <col min="4" max="4" width="20.375" customWidth="1"/>
+    <col min="1" max="1" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.3828125" customWidth="1"/>
+    <col min="3" max="3" width="10.84375" customWidth="1"/>
+    <col min="4" max="4" width="20.3828125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -2110,7 +2131,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>172</v>
       </c>
@@ -2124,7 +2145,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>177</v>
       </c>
@@ -2138,7 +2159,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>182</v>
       </c>
@@ -2152,7 +2173,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>189</v>
       </c>
@@ -2166,7 +2187,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>190</v>
       </c>
@@ -2180,7 +2201,7 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1"/>
+    <hyperlink ref="D9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2193,24 +2214,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D17" sqref="C10:D17"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.765625" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.375" customWidth="1"/>
-    <col min="7" max="7" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.23046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.15234375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.61328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.3828125" customWidth="1"/>
+    <col min="7" max="7" width="9.3828125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>175</v>
       </c>
@@ -2233,7 +2254,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.3">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -2256,7 +2277,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="63" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.3">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -2276,10 +2297,10 @@
         <v>182</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.3">
       <c r="A4" s="18">
         <v>3</v>
       </c>
@@ -2302,7 +2323,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.3">
       <c r="A5" s="18">
         <v>4</v>
       </c>
@@ -2325,7 +2346,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.3">
       <c r="A6" s="18">
         <v>5</v>
       </c>
@@ -2348,7 +2369,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.3">
       <c r="A7" s="18">
         <v>6</v>
       </c>
@@ -2371,7 +2392,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="94.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.3">
       <c r="A8" s="18">
         <v>7</v>
       </c>
@@ -2394,7 +2415,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.3">
       <c r="A9" s="18">
         <v>8</v>
       </c>
@@ -2417,7 +2438,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="220.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="180" x14ac:dyDescent="0.3">
       <c r="A10" s="25">
         <v>9</v>
       </c>
@@ -2434,7 +2455,7 @@
       <c r="F10" s="19"/>
       <c r="G10" s="25"/>
     </row>
-    <row r="11" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.3">
       <c r="A11" s="25">
         <v>10</v>
       </c>
@@ -2451,7 +2472,7 @@
       <c r="F11" s="19"/>
       <c r="G11" s="25"/>
     </row>
-    <row r="12" spans="1:7" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.3">
       <c r="A12" s="25">
         <v>11</v>
       </c>
@@ -2468,7 +2489,7 @@
       <c r="F12" s="19"/>
       <c r="G12" s="25"/>
     </row>
-    <row r="13" spans="1:7" ht="63" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.3">
       <c r="A13" s="18">
         <v>12</v>
       </c>
@@ -2485,7 +2506,7 @@
       <c r="F13" s="19"/>
       <c r="G13" s="18"/>
     </row>
-    <row r="14" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.3">
       <c r="A14" s="18">
         <v>13</v>
       </c>
@@ -2502,7 +2523,7 @@
       <c r="F14" s="19"/>
       <c r="G14" s="18"/>
     </row>
-    <row r="15" spans="1:7" ht="63" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.3">
       <c r="A15" s="18">
         <v>14</v>
       </c>
@@ -2519,7 +2540,7 @@
       <c r="F15" s="19"/>
       <c r="G15" s="18"/>
     </row>
-    <row r="16" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.3">
       <c r="A16" s="18">
         <v>15</v>
       </c>
@@ -2536,7 +2557,7 @@
       <c r="F16" s="19"/>
       <c r="G16" s="18"/>
     </row>
-    <row r="17" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.3">
       <c r="A17" s="18">
         <v>16</v>
       </c>
@@ -2553,7 +2574,7 @@
       <c r="F17" s="19"/>
       <c r="G17" s="18"/>
     </row>
-    <row r="18" spans="1:7" ht="63" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.3">
       <c r="A18" s="18">
         <v>17</v>
       </c>
@@ -2570,7 +2591,7 @@
       <c r="F18" s="19"/>
       <c r="G18" s="18"/>
     </row>
-    <row r="19" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2585,7 +2606,7 @@
       </c>
       <c r="F19" s="19"/>
     </row>
-    <row r="20" spans="1:7" ht="110.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="90" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2600,7 +2621,7 @@
       </c>
       <c r="F20" s="19"/>
     </row>
-    <row r="21" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.3">
       <c r="A21" s="18">
         <v>20</v>
       </c>
@@ -2617,7 +2638,7 @@
       <c r="F21" s="19"/>
       <c r="G21" s="18"/>
     </row>
-    <row r="22" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.3">
       <c r="A22" s="25">
         <v>21</v>
       </c>
@@ -2634,7 +2655,7 @@
       <c r="F22" s="19"/>
       <c r="G22" s="25"/>
     </row>
-    <row r="23" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2649,7 +2670,7 @@
       </c>
       <c r="F23" s="19"/>
     </row>
-    <row r="24" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2664,7 +2685,7 @@
       </c>
       <c r="F24" s="19"/>
     </row>
-    <row r="25" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2679,7 +2700,7 @@
       </c>
       <c r="F25" s="19"/>
     </row>
-    <row r="26" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2694,7 +2715,7 @@
       </c>
       <c r="F26" s="19"/>
     </row>
-    <row r="27" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2709,7 +2730,7 @@
       </c>
       <c r="F27" s="19"/>
     </row>
-    <row r="28" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2724,7 +2745,7 @@
       </c>
       <c r="F28" s="19"/>
     </row>
-    <row r="29" spans="1:7" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2739,7 +2760,7 @@
       </c>
       <c r="F29" s="19"/>
     </row>
-    <row r="30" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2754,7 +2775,7 @@
       </c>
       <c r="F30" s="19"/>
     </row>
-    <row r="31" spans="1:7" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2769,7 +2790,7 @@
       </c>
       <c r="F31" s="19"/>
     </row>
-    <row r="32" spans="1:7" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2784,7 +2805,7 @@
       </c>
       <c r="F32" s="19"/>
     </row>
-    <row r="33" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2800,7 +2821,7 @@
       <c r="F33" s="19"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1"/>
+  <autoFilter ref="A1:F1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <sortState ref="A2:G34">
     <sortCondition ref="A2:A34"/>
   </sortState>
@@ -2816,54 +2837,54 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="7"/>
-    <col min="2" max="2" width="9.375" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.25" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="9.3828125" customWidth="1"/>
+    <col min="3" max="3" width="15.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.23046875" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" customWidth="1"/>
+    <col min="6" max="6" width="12.3828125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>154</v>
       </c>
@@ -2886,7 +2907,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>155</v>
       </c>
@@ -2902,7 +2923,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>156</v>
       </c>
@@ -2927,7 +2948,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>157</v>
       </c>
@@ -2952,7 +2973,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>158</v>
       </c>
@@ -2977,7 +2998,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>159</v>
       </c>
@@ -3015,24 +3036,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11" style="2"/>
-    <col min="3" max="3" width="16.75" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="7.125" customWidth="1"/>
-    <col min="6" max="6" width="6.875" customWidth="1"/>
-    <col min="7" max="7" width="12.375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="16.765625" customWidth="1"/>
+    <col min="4" max="4" width="12.3828125" customWidth="1"/>
+    <col min="5" max="5" width="7.15234375" customWidth="1"/>
+    <col min="6" max="6" width="6.84375" customWidth="1"/>
+    <col min="7" max="7" width="12.3828125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>154</v>
       </c>
@@ -3055,7 +3074,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>155</v>
       </c>
@@ -3068,8 +3087,14 @@
       <c r="E2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>156</v>
       </c>
@@ -3084,14 +3109,56 @@
         <v>8</v>
       </c>
       <c r="E3">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="F3">
-        <v>296</v>
+        <v>235</v>
       </c>
       <c r="G3" s="9">
         <f>(E3-E2)/F3*60</f>
-        <v>19.256756756756758</v>
+        <v>20.170212765957444</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B4" s="2">
+        <v>41717</v>
+      </c>
+      <c r="C4">
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B5" s="2">
+        <v>41731</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B6" s="2">
+        <v>41745</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -3108,27 +3175,25 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.25" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.23046875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.375" style="26" customWidth="1"/>
-    <col min="3" max="3" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.625" customWidth="1"/>
-    <col min="5" max="5" width="24.625" customWidth="1"/>
-    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.25" customWidth="1"/>
-    <col min="8" max="8" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.375" style="6" customWidth="1"/>
+    <col min="1" max="1" width="10.07421875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.84375" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.4609375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.4609375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3157,7 +3222,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>128</v>
       </c>
@@ -3186,7 +3251,7 @@
         <v>41682</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>129</v>
       </c>
@@ -3211,8 +3276,11 @@
       <c r="H3">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I3" s="6">
+        <v>41685</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>122</v>
       </c>
@@ -3241,7 +3309,7 @@
         <v>41678</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>194</v>
       </c>
@@ -3258,7 +3326,7 @@
         <v>41678</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
         <v>195</v>
       </c>
@@ -3275,7 +3343,7 @@
         <v>41678</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>196</v>
       </c>
@@ -3292,7 +3360,7 @@
         <v>41678</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>196</v>
       </c>
@@ -3309,7 +3377,7 @@
         <v>41678</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>107</v>
       </c>
@@ -3338,7 +3406,7 @@
         <v>41681</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>108</v>
       </c>
@@ -3367,7 +3435,7 @@
         <v>41681</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>109</v>
       </c>
@@ -3387,7 +3455,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>113</v>
       </c>
@@ -3416,7 +3484,7 @@
         <v>41680</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="21" t="s">
         <v>201</v>
       </c>
@@ -3433,7 +3501,7 @@
         <v>41680</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="25" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" s="25" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
         <v>202</v>
       </c>
@@ -3450,7 +3518,7 @@
         <v>41680</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
         <v>203</v>
       </c>
@@ -3467,7 +3535,7 @@
         <v>41680</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>127</v>
       </c>
@@ -3487,7 +3555,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="29" t="s">
         <v>209</v>
       </c>
@@ -3513,7 +3581,7 @@
         <v>41685</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A18" s="30" t="s">
         <v>212</v>
       </c>
@@ -3527,7 +3595,7 @@
         <v>41685</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
         <v>214</v>
       </c>
@@ -3541,7 +3609,7 @@
         <v>41685</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A20" s="30" t="s">
         <v>216</v>
       </c>
@@ -3555,7 +3623,7 @@
         <v>41685</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="67.5" x14ac:dyDescent="0.3">
       <c r="A21" s="31" t="s">
         <v>211</v>
       </c>
@@ -3581,27 +3649,27 @@
         <v>41685</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B22" s="28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B23" s="28"/>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B24" s="28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B28" s="28" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I16"/>
+  <autoFilter ref="A1:I16" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3614,19 +3682,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.875" style="32" customWidth="1"/>
+    <col min="2" max="2" width="19.84375" style="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3655,7 +3723,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>132</v>
       </c>
@@ -3663,7 +3731,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>133</v>
       </c>
@@ -3674,7 +3742,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>118</v>
       </c>
@@ -3685,23 +3753,47 @@
         <v>177</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>116</v>
       </c>
       <c r="B5" s="24" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D5" t="s">
+        <v>219</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>115</v>
       </c>
       <c r="B6" s="24" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D6" t="s">
+        <v>219</v>
+      </c>
+      <c r="E6">
+        <v>30</v>
+      </c>
+      <c r="F6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>110</v>
       </c>
@@ -3709,7 +3801,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>111</v>
       </c>
@@ -3717,7 +3809,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>112</v>
       </c>
@@ -3738,16 +3830,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3788,16 +3880,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3838,18 +3930,20 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.15234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.3828125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>106</v>
       </c>
@@ -3860,7 +3954,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -3871,7 +3965,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -3882,7 +3976,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -3893,7 +3987,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -3904,7 +3998,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>111</v>
       </c>
@@ -3915,7 +4009,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -3926,7 +4020,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>113</v>
       </c>
@@ -3937,7 +4031,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -3948,7 +4042,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>115</v>
       </c>
@@ -3959,7 +4053,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>116</v>
       </c>
@@ -3970,7 +4064,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>117</v>
       </c>
@@ -3981,7 +4075,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>118</v>
       </c>
@@ -3992,7 +4086,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>119</v>
       </c>
@@ -4003,7 +4097,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>120</v>
       </c>
@@ -4014,7 +4108,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>121</v>
       </c>
@@ -4025,7 +4119,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>122</v>
       </c>
@@ -4036,7 +4130,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>123</v>
       </c>
@@ -4047,7 +4141,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>124</v>
       </c>
@@ -4058,7 +4152,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>125</v>
       </c>
@@ -4069,7 +4163,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>126</v>
       </c>
@@ -4080,7 +4174,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>127</v>
       </c>
@@ -4091,7 +4185,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>128</v>
       </c>
@@ -4102,7 +4196,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>129</v>
       </c>
@@ -4113,7 +4207,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>130</v>
       </c>
@@ -4124,7 +4218,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>131</v>
       </c>
@@ -4135,7 +4229,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="126" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>132</v>
       </c>
@@ -4146,7 +4240,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>133</v>
       </c>
@@ -4157,7 +4251,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>134</v>
       </c>
@@ -4168,7 +4262,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>135</v>
       </c>
@@ -4179,7 +4273,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>136</v>
       </c>
@@ -4190,7 +4284,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>137</v>
       </c>
@@ -4201,7 +4295,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>138</v>
       </c>
@@ -4212,7 +4306,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>139</v>
       </c>
@@ -4223,7 +4317,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>140</v>
       </c>
@@ -4234,7 +4328,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>141</v>
       </c>
@@ -4245,7 +4339,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>142</v>
       </c>
@@ -4256,7 +4350,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>143</v>
       </c>
@@ -4267,7 +4361,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>144</v>
       </c>
@@ -4278,7 +4372,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>145</v>
       </c>
@@ -4289,7 +4383,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>146</v>
       </c>
@@ -4300,7 +4394,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>147</v>
       </c>
@@ -4311,7 +4405,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>148</v>
       </c>

</xml_diff>

<commit_message>
Updated status with completion of US21
</commit_message>
<xml_diff>
--- a/TeamEstherKarelKeithTroyReport.xlsx
+++ b/TeamEstherKarelKeithTroyReport.xlsx
@@ -2218,7 +2218,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.765625" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -2435,7 +2435,7 @@
         <v>182</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>192</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="180" x14ac:dyDescent="0.3">
@@ -3109,14 +3109,14 @@
         <v>8</v>
       </c>
       <c r="E3">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="F3">
-        <v>235</v>
+        <v>295</v>
       </c>
       <c r="G3" s="9">
         <f>(E3-E2)/F3*60</f>
-        <v>20.170212765957444</v>
+        <v>19.525423728813557</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -3554,6 +3554,15 @@
       <c r="F16">
         <v>30</v>
       </c>
+      <c r="G16">
+        <v>17</v>
+      </c>
+      <c r="H16">
+        <v>60</v>
+      </c>
+      <c r="I16" s="6">
+        <v>41687</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="29" t="s">

</xml_diff>

<commit_message>
Updated backlog tracking data
</commit_message>
<xml_diff>
--- a/TeamEstherKarelKeithTroyReport.xlsx
+++ b/TeamEstherKarelKeithTroyReport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="16430" tabRatio="627" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="16430" tabRatio="627" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="221">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -720,6 +720,9 @@
   </si>
   <si>
     <t>not started</t>
+  </si>
+  <si>
+    <t>Not Started</t>
   </si>
 </sst>
 </file>
@@ -861,7 +864,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -926,6 +929,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="68" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="68" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="68" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="71">
@@ -2215,10 +2230,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.765625" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -2228,10 +2243,12 @@
     <col min="3" max="3" width="10.15234375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.61328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.3828125" customWidth="1"/>
-    <col min="7" max="7" width="9.3828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.765625" style="34" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.84375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.23046875" style="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>175</v>
       </c>
@@ -2247,14 +2264,17 @@
       <c r="E1" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="35" t="s">
         <v>170</v>
       </c>
       <c r="G1" s="17" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.3">
+      <c r="H1" s="33" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -2270,14 +2290,17 @@
       <c r="E2" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="34" t="s">
         <v>172</v>
       </c>
       <c r="G2" s="20" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.3">
+      <c r="H2" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -2293,14 +2316,17 @@
       <c r="E3" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="34" t="s">
         <v>182</v>
       </c>
       <c r="G3" s="20" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.3">
+      <c r="H3" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A4" s="18">
         <v>3</v>
       </c>
@@ -2316,14 +2342,17 @@
       <c r="E4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="34" t="s">
         <v>177</v>
       </c>
       <c r="G4" s="20" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.3">
+      <c r="H4" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A5" s="18">
         <v>4</v>
       </c>
@@ -2339,14 +2368,17 @@
       <c r="E5" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="34" t="s">
         <v>189</v>
       </c>
       <c r="G5" s="20" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.3">
+      <c r="H5" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A6" s="18">
         <v>5</v>
       </c>
@@ -2362,14 +2394,17 @@
       <c r="E6" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="34" t="s">
         <v>189</v>
       </c>
       <c r="G6" s="20" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.3">
+      <c r="H6" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A7" s="18">
         <v>6</v>
       </c>
@@ -2385,14 +2420,17 @@
       <c r="E7" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="34" t="s">
         <v>172</v>
       </c>
       <c r="G7" s="20" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.3">
+      <c r="H7" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.3">
       <c r="A8" s="18">
         <v>7</v>
       </c>
@@ -2408,14 +2446,17 @@
       <c r="E8" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="34" t="s">
         <v>177</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.3">
+      <c r="H8" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A9" s="18">
         <v>8</v>
       </c>
@@ -2431,14 +2472,17 @@
       <c r="E9" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="34" t="s">
         <v>182</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="180" x14ac:dyDescent="0.3">
+      <c r="H9" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="180" x14ac:dyDescent="0.3">
       <c r="A10" s="25">
         <v>9</v>
       </c>
@@ -2452,10 +2496,13 @@
       <c r="E10" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="F10" s="19"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="25"/>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.3">
+      <c r="H10" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A11" s="25">
         <v>10</v>
       </c>
@@ -2469,10 +2516,15 @@
       <c r="E11" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="19"/>
+      <c r="F11" s="36" t="s">
+        <v>177</v>
+      </c>
       <c r="G11" s="25"/>
-    </row>
-    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.3">
+      <c r="H11" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A12" s="25">
         <v>11</v>
       </c>
@@ -2486,10 +2538,15 @@
       <c r="E12" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="19"/>
+      <c r="F12" s="36" t="s">
+        <v>177</v>
+      </c>
       <c r="G12" s="25"/>
-    </row>
-    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.3">
+      <c r="H12" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A13" s="18">
         <v>12</v>
       </c>
@@ -2503,10 +2560,17 @@
       <c r="E13" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="F13" s="19"/>
-      <c r="G13" s="18"/>
-    </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.3">
+      <c r="F13" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="H13" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A14" s="18">
         <v>13</v>
       </c>
@@ -2520,10 +2584,17 @@
       <c r="E14" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="19"/>
-      <c r="G14" s="18"/>
-    </row>
-    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.3">
+      <c r="F14" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="H14" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A15" s="18">
         <v>14</v>
       </c>
@@ -2537,10 +2608,13 @@
       <c r="E15" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="19"/>
+      <c r="F15" s="36"/>
       <c r="G15" s="18"/>
-    </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.3">
+      <c r="H15" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A16" s="18">
         <v>15</v>
       </c>
@@ -2554,10 +2628,13 @@
       <c r="E16" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="19"/>
+      <c r="F16" s="36"/>
       <c r="G16" s="18"/>
-    </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.3">
+      <c r="H16" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A17" s="18">
         <v>16</v>
       </c>
@@ -2571,10 +2648,13 @@
       <c r="E17" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="19"/>
+      <c r="F17" s="36"/>
       <c r="G17" s="18"/>
-    </row>
-    <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.3">
+      <c r="H17" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A18" s="18">
         <v>17</v>
       </c>
@@ -2588,10 +2668,13 @@
       <c r="E18" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="F18" s="19"/>
+      <c r="F18" s="36"/>
       <c r="G18" s="18"/>
-    </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.3">
+      <c r="H18" s="34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2604,9 +2687,12 @@
       <c r="E19" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="F19" s="19"/>
-    </row>
-    <row r="20" spans="1:7" ht="90" x14ac:dyDescent="0.3">
+      <c r="F19" s="36"/>
+      <c r="H19" s="34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="90" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2619,9 +2705,12 @@
       <c r="E20" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="F20" s="19"/>
-    </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.3">
+      <c r="F20" s="36"/>
+      <c r="H20" s="34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A21" s="18">
         <v>20</v>
       </c>
@@ -2635,10 +2724,13 @@
       <c r="E21" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="19"/>
+      <c r="F21" s="36"/>
       <c r="G21" s="18"/>
-    </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.3">
+      <c r="H21" s="34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A22" s="25">
         <v>21</v>
       </c>
@@ -2652,10 +2744,13 @@
       <c r="E22" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F22" s="19"/>
+      <c r="F22" s="36"/>
       <c r="G22" s="25"/>
-    </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.3">
+      <c r="H22" s="34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2668,9 +2763,12 @@
       <c r="E23" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="F23" s="19"/>
-    </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.3">
+      <c r="F23" s="36"/>
+      <c r="H23" s="34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2683,9 +2781,12 @@
       <c r="E24" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="19"/>
-    </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.3">
+      <c r="F24" s="36"/>
+      <c r="H24" s="34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2698,9 +2799,12 @@
       <c r="E25" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="F25" s="19"/>
-    </row>
-    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.3">
+      <c r="F25" s="36"/>
+      <c r="H25" s="34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2713,9 +2817,12 @@
       <c r="E26" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="19"/>
-    </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.3">
+      <c r="F26" s="36"/>
+      <c r="H26" s="34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2728,9 +2835,12 @@
       <c r="E27" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="19"/>
-    </row>
-    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.3">
+      <c r="F27" s="36"/>
+      <c r="H27" s="34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2743,9 +2853,12 @@
       <c r="E28" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="F28" s="19"/>
-    </row>
-    <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.3">
+      <c r="F28" s="36"/>
+      <c r="H28" s="34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="60" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2758,9 +2871,12 @@
       <c r="E29" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="F29" s="19"/>
-    </row>
-    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.3">
+      <c r="F29" s="36"/>
+      <c r="H29" s="34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2773,9 +2889,12 @@
       <c r="E30" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F30" s="19"/>
-    </row>
-    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.3">
+      <c r="F30" s="36"/>
+      <c r="H30" s="34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2788,9 +2907,12 @@
       <c r="E31" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="F31" s="19"/>
-    </row>
-    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.3">
+      <c r="F31" s="36"/>
+      <c r="H31" s="34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2803,9 +2925,12 @@
       <c r="E32" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="F32" s="19"/>
-    </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.3">
+      <c r="F32" s="36"/>
+      <c r="H32" s="34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2818,7 +2943,10 @@
       <c r="E33" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="F33" s="19"/>
+      <c r="F33" s="36"/>
+      <c r="H33" s="34">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
@@ -3039,7 +3167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
Committing story 05 code and tests
</commit_message>
<xml_diff>
--- a/TeamEstherKarelKeithTroyReport.xlsx
+++ b/TeamEstherKarelKeithTroyReport.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klros\Google Drive\Keith\Stevens Institute of Technology\SSW-555-WS\gedcom\stevens_cs555\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KLahmy\Documents\stevens\CS-555\project\GIT\stevens_cs555\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="16430" tabRatio="627" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-24" windowWidth="28800" windowHeight="16428" tabRatio="627" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backlog!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sprint1!$A$1:$I$16</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="221">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -728,7 +728,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -1014,7 +1014,7 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="68" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="Normal 2" xfId="68"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1030,7 +1030,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1101,7 +1101,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8005-41C3-A2A6-994BE20B6C54}"/>
             </c:ext>
@@ -1117,11 +1117,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="61242752"/>
-        <c:axId val="61269120"/>
+        <c:axId val="87705992"/>
+        <c:axId val="87691520"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="61242752"/>
+        <c:axId val="87705992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1131,14 +1131,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61269120"/>
+        <c:crossAx val="87691520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="61269120"/>
+        <c:axId val="87691520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1149,7 +1149,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61242752"/>
+        <c:crossAx val="87705992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1167,7 +1167,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1238,7 +1238,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5A9F-42BD-9352-89747C7C9AC0}"/>
             </c:ext>
@@ -1254,11 +1254,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="129753856"/>
-        <c:axId val="129755392"/>
+        <c:axId val="88195864"/>
+        <c:axId val="88196248"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="129753856"/>
+        <c:axId val="88195864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1268,14 +1268,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129755392"/>
+        <c:crossAx val="88196248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="129755392"/>
+        <c:axId val="88196248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1286,7 +1286,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129753856"/>
+        <c:crossAx val="88195864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1323,7 +1323,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1361,7 +1361,7 @@
         <xdr:cNvPr id="3" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1436,7 +1436,7 @@
         <xdr:cNvPr id="4" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1501,7 +1501,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1570,7 +1570,7 @@
         <xdr:cNvPr id="6" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1640,7 +1640,7 @@
         <xdr:cNvPr id="7" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1709,7 +1709,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1779,7 +1779,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2119,20 +2119,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.84375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.3828125" customWidth="1"/>
-    <col min="3" max="3" width="10.84375" customWidth="1"/>
-    <col min="4" max="4" width="20.3828125" customWidth="1"/>
+    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.36328125" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" customWidth="1"/>
+    <col min="4" max="4" width="20.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>172</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>177</v>
       </c>
@@ -2174,7 +2174,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>182</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>189</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>190</v>
       </c>
@@ -2216,7 +2216,7 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D9" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2229,26 +2229,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.765625" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.3828125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.23046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.15234375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.61328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.3828125" customWidth="1"/>
-    <col min="6" max="6" width="8.765625" style="34" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.84375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.23046875" style="34" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.36328125" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" style="34" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.26953125" style="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>175</v>
       </c>
@@ -2274,7 +2274,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -2300,7 +2300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="18">
         <v>3</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A5" s="18">
         <v>4</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="18">
         <v>5</v>
       </c>
@@ -2404,7 +2404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" s="18">
         <v>6</v>
       </c>
@@ -2430,7 +2430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.2">
       <c r="A8" s="18">
         <v>7</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A9" s="18">
         <v>8</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="180" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="180" x14ac:dyDescent="0.2">
       <c r="A10" s="25">
         <v>9</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="25">
         <v>10</v>
       </c>
@@ -2524,7 +2524,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A12" s="25">
         <v>11</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A13" s="18">
         <v>12</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" s="18">
         <v>13</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A15" s="18">
         <v>14</v>
       </c>
@@ -2614,7 +2614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" s="18">
         <v>15</v>
       </c>
@@ -2628,13 +2628,15 @@
       <c r="E16" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="36"/>
+      <c r="F16" s="36" t="s">
+        <v>189</v>
+      </c>
       <c r="G16" s="18"/>
       <c r="H16" s="34">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" s="18">
         <v>16</v>
       </c>
@@ -2648,13 +2650,15 @@
       <c r="E17" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="36"/>
+      <c r="F17" s="36" t="s">
+        <v>189</v>
+      </c>
       <c r="G17" s="18"/>
       <c r="H17" s="34">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A18" s="18">
         <v>17</v>
       </c>
@@ -2674,7 +2678,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2692,7 +2696,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="90" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="90" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2710,7 +2714,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" s="18">
         <v>20</v>
       </c>
@@ -2730,7 +2734,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="25">
         <v>21</v>
       </c>
@@ -2750,7 +2754,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2768,7 +2772,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2786,7 +2790,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2804,7 +2808,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2822,7 +2826,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2840,7 +2844,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2858,7 +2862,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="60" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2876,7 +2880,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2894,7 +2898,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2912,7 +2916,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2930,7 +2934,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2949,7 +2953,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:F1"/>
   <sortState ref="A2:G34">
     <sortCondition ref="A2:A34"/>
   </sortState>
@@ -2965,54 +2969,54 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="7"/>
-    <col min="2" max="2" width="9.3828125" customWidth="1"/>
-    <col min="3" max="3" width="15.84375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.23046875" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="12.3828125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="9.36328125" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.36328125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>154</v>
       </c>
@@ -3035,7 +3039,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>155</v>
       </c>
@@ -3051,7 +3055,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>156</v>
       </c>
@@ -3076,7 +3080,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>157</v>
       </c>
@@ -3101,7 +3105,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>158</v>
       </c>
@@ -3126,7 +3130,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>159</v>
       </c>
@@ -3164,22 +3168,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11" style="2"/>
-    <col min="3" max="3" width="16.765625" customWidth="1"/>
-    <col min="4" max="4" width="12.3828125" customWidth="1"/>
-    <col min="5" max="5" width="7.15234375" customWidth="1"/>
-    <col min="6" max="6" width="6.84375" customWidth="1"/>
-    <col min="7" max="7" width="12.3828125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="16.7265625" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="7.1796875" customWidth="1"/>
+    <col min="6" max="6" width="6.81640625" customWidth="1"/>
+    <col min="7" max="7" width="12.36328125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>154</v>
       </c>
@@ -3202,7 +3206,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>155</v>
       </c>
@@ -3222,7 +3226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>156</v>
       </c>
@@ -3247,7 +3251,7 @@
         <v>19.525423728813557</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>157</v>
       </c>
@@ -3261,7 +3265,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>158</v>
       </c>
@@ -3275,7 +3279,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>159</v>
       </c>
@@ -3303,25 +3307,25 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.23046875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.26953125" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.07421875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.84375" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.4609375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.4609375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.81640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.453125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3350,7 +3354,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>128</v>
       </c>
@@ -3379,7 +3383,7 @@
         <v>41682</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
         <v>129</v>
       </c>
@@ -3408,7 +3412,7 @@
         <v>41685</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>122</v>
       </c>
@@ -3437,7 +3441,7 @@
         <v>41678</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
         <v>194</v>
       </c>
@@ -3454,7 +3458,7 @@
         <v>41678</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
         <v>195</v>
       </c>
@@ -3471,7 +3475,7 @@
         <v>41678</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
         <v>196</v>
       </c>
@@ -3488,7 +3492,7 @@
         <v>41678</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
         <v>196</v>
       </c>
@@ -3505,7 +3509,7 @@
         <v>41678</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
         <v>107</v>
       </c>
@@ -3534,7 +3538,7 @@
         <v>41681</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
         <v>108</v>
       </c>
@@ -3563,7 +3567,7 @@
         <v>41681</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
         <v>109</v>
       </c>
@@ -3583,7 +3587,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
         <v>113</v>
       </c>
@@ -3612,7 +3616,7 @@
         <v>41680</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="21" t="s">
         <v>201</v>
       </c>
@@ -3629,7 +3633,7 @@
         <v>41680</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="25" customFormat="1" ht="27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" s="25" customFormat="1" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="s">
         <v>202</v>
       </c>
@@ -3646,7 +3650,7 @@
         <v>41680</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
         <v>203</v>
       </c>
@@ -3663,7 +3667,7 @@
         <v>41680</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
         <v>127</v>
       </c>
@@ -3692,7 +3696,7 @@
         <v>41687</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="29" t="s">
         <v>209</v>
       </c>
@@ -3718,7 +3722,7 @@
         <v>41685</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A18" s="30" t="s">
         <v>212</v>
       </c>
@@ -3732,7 +3736,7 @@
         <v>41685</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A19" s="30" t="s">
         <v>214</v>
       </c>
@@ -3746,7 +3750,7 @@
         <v>41685</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="A20" s="30" t="s">
         <v>216</v>
       </c>
@@ -3760,7 +3764,7 @@
         <v>41685</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="63" x14ac:dyDescent="0.2">
       <c r="A21" s="31" t="s">
         <v>211</v>
       </c>
@@ -3786,27 +3790,27 @@
         <v>41685</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B22" s="28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B23" s="28"/>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B24" s="28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B28" s="28" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I16" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
+  <autoFilter ref="A1:I16"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3819,19 +3823,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.84375" style="32" customWidth="1"/>
+    <col min="2" max="2" width="19.81640625" style="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3860,7 +3864,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>132</v>
       </c>
@@ -3868,7 +3872,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
         <v>133</v>
       </c>
@@ -3879,7 +3883,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>118</v>
       </c>
@@ -3890,7 +3894,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
         <v>116</v>
       </c>
@@ -3910,7 +3914,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
         <v>115</v>
       </c>
@@ -3930,7 +3934,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
         <v>110</v>
       </c>
@@ -3938,7 +3942,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
         <v>111</v>
       </c>
@@ -3946,7 +3950,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
         <v>112</v>
       </c>
@@ -3967,16 +3971,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4017,16 +4021,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4067,20 +4071,20 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.3828125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.36328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>106</v>
       </c>
@@ -4091,7 +4095,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -4102,7 +4106,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -4113,7 +4117,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -4124,7 +4128,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -4135,7 +4139,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>111</v>
       </c>
@@ -4146,7 +4150,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -4157,7 +4161,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>113</v>
       </c>
@@ -4168,7 +4172,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -4179,7 +4183,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>115</v>
       </c>
@@ -4190,7 +4194,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>116</v>
       </c>
@@ -4201,7 +4205,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>117</v>
       </c>
@@ -4212,7 +4216,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>118</v>
       </c>
@@ -4223,7 +4227,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>119</v>
       </c>
@@ -4234,7 +4238,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>120</v>
       </c>
@@ -4245,7 +4249,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>121</v>
       </c>
@@ -4256,7 +4260,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>122</v>
       </c>
@@ -4267,7 +4271,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>123</v>
       </c>
@@ -4278,7 +4282,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>124</v>
       </c>
@@ -4289,7 +4293,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>125</v>
       </c>
@@ -4300,7 +4304,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>126</v>
       </c>
@@ -4311,7 +4315,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>127</v>
       </c>
@@ -4322,7 +4326,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>128</v>
       </c>
@@ -4333,7 +4337,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>129</v>
       </c>
@@ -4344,7 +4348,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>130</v>
       </c>
@@ -4355,7 +4359,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>131</v>
       </c>
@@ -4366,7 +4370,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>132</v>
       </c>
@@ -4377,7 +4381,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>133</v>
       </c>
@@ -4388,7 +4392,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>134</v>
       </c>
@@ -4399,7 +4403,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>135</v>
       </c>
@@ -4410,7 +4414,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>136</v>
       </c>
@@ -4421,7 +4425,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>137</v>
       </c>
@@ -4432,7 +4436,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>138</v>
       </c>
@@ -4443,7 +4447,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>139</v>
       </c>
@@ -4454,7 +4458,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>140</v>
       </c>
@@ -4465,7 +4469,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>141</v>
       </c>
@@ -4476,7 +4480,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>142</v>
       </c>
@@ -4487,7 +4491,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>143</v>
       </c>
@@ -4498,7 +4502,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>144</v>
       </c>
@@ -4509,7 +4513,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>145</v>
       </c>
@@ -4520,7 +4524,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>146</v>
       </c>
@@ -4531,7 +4535,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>147</v>
       </c>
@@ -4542,7 +4546,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>148</v>
       </c>

</xml_diff>

<commit_message>
Changes for story 5/6
</commit_message>
<xml_diff>
--- a/TeamEstherKarelKeithTroyReport.xlsx
+++ b/TeamEstherKarelKeithTroyReport.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="221">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1117,11 +1117,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="87705992"/>
-        <c:axId val="87691520"/>
+        <c:axId val="159963320"/>
+        <c:axId val="159963712"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="87705992"/>
+        <c:axId val="159963320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1131,14 +1131,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87691520"/>
+        <c:crossAx val="159963712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="87691520"/>
+        <c:axId val="159963712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1149,7 +1149,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87705992"/>
+        <c:crossAx val="159963320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1254,11 +1254,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="88195864"/>
-        <c:axId val="88196248"/>
+        <c:axId val="159965280"/>
+        <c:axId val="159965672"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="88195864"/>
+        <c:axId val="159965280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1268,14 +1268,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88196248"/>
+        <c:crossAx val="159965672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="88196248"/>
+        <c:axId val="159965672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1286,7 +1286,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88195864"/>
+        <c:crossAx val="159965280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1323,7 +1323,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1361,7 +1361,7 @@
         <xdr:cNvPr id="3" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1436,7 +1436,7 @@
         <xdr:cNvPr id="4" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1501,7 +1501,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1570,7 +1570,7 @@
         <xdr:cNvPr id="6" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1640,7 +1640,7 @@
         <xdr:cNvPr id="7" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1709,7 +1709,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1779,7 +1779,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2232,8 +2232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -2631,7 +2631,9 @@
       <c r="F16" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="G16" s="18"/>
+      <c r="G16" s="20" t="s">
+        <v>207</v>
+      </c>
       <c r="H16" s="34">
         <v>2</v>
       </c>
@@ -2653,7 +2655,9 @@
       <c r="F17" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="G17" s="18"/>
+      <c r="G17" s="20" t="s">
+        <v>207</v>
+      </c>
       <c r="H17" s="34">
         <v>2</v>
       </c>

</xml_diff>